<commit_message>
[0406] Get imported time
</commit_message>
<xml_diff>
--- a/src/main/resources/static/document/Template Cow Import.xlsx
+++ b/src/main/resources/static/document/Template Cow Import.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9000" activeTab="2"/>
+    <workbookView windowWidth="23040" windowHeight="9000"/>
   </bookViews>
   <sheets>
     <sheet name="Import time" sheetId="1" r:id="rId1"/>
@@ -562,7 +562,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -582,6 +582,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -707,7 +722,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -719,34 +734,34 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -848,8 +863,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="178" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1325,21 +1340,21 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6296296296296" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="12.6296296296296" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1"/>
   <sheetData>
-    <row r="1" customHeight="1" spans="1:2">
+    <row r="1" customHeight="1" spans="1:1">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15">
-        <v>1</v>
-      </c>
+    </row>
+    <row r="2" customHeight="1" spans="1:1">
+      <c r="A2" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1355,7 +1370,7 @@
   <dimension ref="A1:K300"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6296296296296" defaultRowHeight="15.75" customHeight="1"/>
@@ -1391,7 +1406,7 @@
     </row>
     <row r="2" customHeight="1" spans="1:8">
       <c r="A2" s="12" t="str">
-        <f>IF(G2&lt;&gt;"",UPPER(LEFT(G2,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G2,G2),"0000"),"")</f>
+        <f>IF(G2&lt;&gt;"",UPPER(LEFT(G2,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G2,G2),"0000"),"")</f>
         <v/>
       </c>
       <c r="B2" s="6"/>
@@ -1404,7 +1419,7 @@
     </row>
     <row r="3" customHeight="1" spans="1:8">
       <c r="A3" s="12" t="str">
-        <f>IF(G3&lt;&gt;"",UPPER(LEFT(G3,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G3,G3),"0000"),"")</f>
+        <f>IF(G3&lt;&gt;"",UPPER(LEFT(G3,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G3,G3),"0000"),"")</f>
         <v/>
       </c>
       <c r="B3" s="6"/>
@@ -1417,7 +1432,7 @@
     </row>
     <row r="4" customHeight="1" spans="1:8">
       <c r="A4" s="12" t="str">
-        <f>IF(G4&lt;&gt;"",UPPER(LEFT(G4,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G4,G4),"0000"),"")</f>
+        <f>IF(G4&lt;&gt;"",UPPER(LEFT(G4,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G4,G4),"0000"),"")</f>
         <v/>
       </c>
       <c r="B4" s="6"/>
@@ -1430,7 +1445,7 @@
     </row>
     <row r="5" customHeight="1" spans="1:8">
       <c r="A5" s="12" t="str">
-        <f>IF(G5&lt;&gt;"",UPPER(LEFT(G5,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G5,G5),"0000"),"")</f>
+        <f>IF(G5&lt;&gt;"",UPPER(LEFT(G5,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G5,G5),"0000"),"")</f>
         <v/>
       </c>
       <c r="B5" s="6"/>
@@ -1443,7 +1458,7 @@
     </row>
     <row r="6" customHeight="1" spans="1:8">
       <c r="A6" s="12" t="str">
-        <f>IF(G6&lt;&gt;"",UPPER(LEFT(G6,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G6,G6),"0000"),"")</f>
+        <f>IF(G6&lt;&gt;"",UPPER(LEFT(G6,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G6,G6),"0000"),"")</f>
         <v/>
       </c>
       <c r="B6" s="6"/>
@@ -1456,7 +1471,7 @@
     </row>
     <row r="7" customHeight="1" spans="1:11">
       <c r="A7" s="12" t="str">
-        <f>IF(G7&lt;&gt;"",UPPER(LEFT(G7,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G7,G7),"0000"),"")</f>
+        <f>IF(G7&lt;&gt;"",UPPER(LEFT(G7,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G7,G7),"0000"),"")</f>
         <v/>
       </c>
       <c r="B7" s="6"/>
@@ -1471,7 +1486,7 @@
     </row>
     <row r="8" customHeight="1" spans="1:11">
       <c r="A8" s="12" t="str">
-        <f>IF(G8&lt;&gt;"",UPPER(LEFT(G8,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G8,G8),"0000"),"")</f>
+        <f>IF(G8&lt;&gt;"",UPPER(LEFT(G8,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G8,G8),"0000"),"")</f>
         <v/>
       </c>
       <c r="B8" s="6"/>
@@ -1485,7 +1500,7 @@
     </row>
     <row r="9" customHeight="1" spans="1:8">
       <c r="A9" s="12" t="str">
-        <f>IF(G9&lt;&gt;"",UPPER(LEFT(G9,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G9,G9),"0000"),"")</f>
+        <f>IF(G9&lt;&gt;"",UPPER(LEFT(G9,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G9,G9),"0000"),"")</f>
         <v/>
       </c>
       <c r="B9" s="6"/>
@@ -1498,7 +1513,7 @@
     </row>
     <row r="10" customHeight="1" spans="1:8">
       <c r="A10" s="12" t="str">
-        <f>IF(G10&lt;&gt;"",UPPER(LEFT(G10,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G10,G10),"0000"),"")</f>
+        <f>IF(G10&lt;&gt;"",UPPER(LEFT(G10,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G10,G10),"0000"),"")</f>
         <v/>
       </c>
       <c r="B10" s="6"/>
@@ -1511,7 +1526,7 @@
     </row>
     <row r="11" customHeight="1" spans="1:8">
       <c r="A11" s="12" t="str">
-        <f>IF(G11&lt;&gt;"",UPPER(LEFT(G11,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G11,G11),"0000"),"")</f>
+        <f>IF(G11&lt;&gt;"",UPPER(LEFT(G11,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G11,G11),"0000"),"")</f>
         <v/>
       </c>
       <c r="B11" s="6"/>
@@ -1524,7 +1539,7 @@
     </row>
     <row r="12" customHeight="1" spans="1:8">
       <c r="A12" s="12" t="str">
-        <f>IF(G12&lt;&gt;"",UPPER(LEFT(G12,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G12,G12),"0000"),"")</f>
+        <f>IF(G12&lt;&gt;"",UPPER(LEFT(G12,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G12,G12),"0000"),"")</f>
         <v/>
       </c>
       <c r="B12" s="5"/>
@@ -1537,7 +1552,7 @@
     </row>
     <row r="13" customHeight="1" spans="1:8">
       <c r="A13" s="12" t="str">
-        <f>IF(G13&lt;&gt;"",UPPER(LEFT(G13,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G13,G13),"0000"),"")</f>
+        <f>IF(G13&lt;&gt;"",UPPER(LEFT(G13,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G13,G13),"0000"),"")</f>
         <v/>
       </c>
       <c r="B13" s="5"/>
@@ -1550,7 +1565,7 @@
     </row>
     <row r="14" customHeight="1" spans="1:8">
       <c r="A14" s="12" t="str">
-        <f>IF(G14&lt;&gt;"",UPPER(LEFT(G14,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G14,G14),"0000"),"")</f>
+        <f>IF(G14&lt;&gt;"",UPPER(LEFT(G14,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G14,G14),"0000"),"")</f>
         <v/>
       </c>
       <c r="B14" s="5"/>
@@ -1563,7 +1578,7 @@
     </row>
     <row r="15" customHeight="1" spans="1:8">
       <c r="A15" s="12" t="str">
-        <f>IF(G15&lt;&gt;"",UPPER(LEFT(G15,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G15,G15),"0000"),"")</f>
+        <f>IF(G15&lt;&gt;"",UPPER(LEFT(G15,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G15,G15),"0000"),"")</f>
         <v/>
       </c>
       <c r="B15" s="5"/>
@@ -1576,7 +1591,7 @@
     </row>
     <row r="16" customHeight="1" spans="1:8">
       <c r="A16" s="12" t="str">
-        <f>IF(G16&lt;&gt;"",UPPER(LEFT(G16,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G16,G16),"0000"),"")</f>
+        <f>IF(G16&lt;&gt;"",UPPER(LEFT(G16,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G16,G16),"0000"),"")</f>
         <v/>
       </c>
       <c r="B16" s="5"/>
@@ -1589,7 +1604,7 @@
     </row>
     <row r="17" customHeight="1" spans="1:8">
       <c r="A17" s="12" t="str">
-        <f>IF(G17&lt;&gt;"",UPPER(LEFT(G17,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G17,G17),"0000"),"")</f>
+        <f>IF(G17&lt;&gt;"",UPPER(LEFT(G17,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G17,G17),"0000"),"")</f>
         <v/>
       </c>
       <c r="B17" s="5"/>
@@ -1602,7 +1617,7 @@
     </row>
     <row r="18" customHeight="1" spans="1:8">
       <c r="A18" s="12" t="str">
-        <f>IF(G18&lt;&gt;"",UPPER(LEFT(G18,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G18,G18),"0000"),"")</f>
+        <f>IF(G18&lt;&gt;"",UPPER(LEFT(G18,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G18,G18),"0000"),"")</f>
         <v/>
       </c>
       <c r="B18" s="5"/>
@@ -1615,7 +1630,7 @@
     </row>
     <row r="19" customHeight="1" spans="1:8">
       <c r="A19" s="12" t="str">
-        <f>IF(G19&lt;&gt;"",UPPER(LEFT(G19,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G19,G19),"0000"),"")</f>
+        <f>IF(G19&lt;&gt;"",UPPER(LEFT(G19,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G19,G19),"0000"),"")</f>
         <v/>
       </c>
       <c r="B19" s="5"/>
@@ -1628,7 +1643,7 @@
     </row>
     <row r="20" customHeight="1" spans="1:8">
       <c r="A20" s="12" t="str">
-        <f>IF(G20&lt;&gt;"",UPPER(LEFT(G20,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G20,G20),"0000"),"")</f>
+        <f>IF(G20&lt;&gt;"",UPPER(LEFT(G20,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G20,G20),"0000"),"")</f>
         <v/>
       </c>
       <c r="B20" s="5"/>
@@ -1641,7 +1656,7 @@
     </row>
     <row r="21" customHeight="1" spans="1:8">
       <c r="A21" s="12" t="str">
-        <f>IF(G21&lt;&gt;"",UPPER(LEFT(G21,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G21,G21),"0000"),"")</f>
+        <f>IF(G21&lt;&gt;"",UPPER(LEFT(G21,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G21,G21),"0000"),"")</f>
         <v/>
       </c>
       <c r="B21" s="5"/>
@@ -1654,7 +1669,7 @@
     </row>
     <row r="22" customHeight="1" spans="1:8">
       <c r="A22" s="12" t="str">
-        <f>IF(G22&lt;&gt;"",UPPER(LEFT(G22,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G22,G22),"0000"),"")</f>
+        <f>IF(G22&lt;&gt;"",UPPER(LEFT(G22,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G22,G22),"0000"),"")</f>
         <v/>
       </c>
       <c r="B22" s="5"/>
@@ -1667,7 +1682,7 @@
     </row>
     <row r="23" customHeight="1" spans="1:8">
       <c r="A23" s="12" t="str">
-        <f>IF(G23&lt;&gt;"",UPPER(LEFT(G23,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G23,G23),"0000"),"")</f>
+        <f>IF(G23&lt;&gt;"",UPPER(LEFT(G23,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G23,G23),"0000"),"")</f>
         <v/>
       </c>
       <c r="B23" s="5"/>
@@ -1680,7 +1695,7 @@
     </row>
     <row r="24" customHeight="1" spans="1:8">
       <c r="A24" s="12" t="str">
-        <f>IF(G24&lt;&gt;"",UPPER(LEFT(G24,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G24,G24),"0000"),"")</f>
+        <f>IF(G24&lt;&gt;"",UPPER(LEFT(G24,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G24,G24),"0000"),"")</f>
         <v/>
       </c>
       <c r="B24" s="5"/>
@@ -1693,7 +1708,7 @@
     </row>
     <row r="25" customHeight="1" spans="1:8">
       <c r="A25" s="12" t="str">
-        <f>IF(G25&lt;&gt;"",UPPER(LEFT(G25,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G25,G25),"0000"),"")</f>
+        <f>IF(G25&lt;&gt;"",UPPER(LEFT(G25,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G25,G25),"0000"),"")</f>
         <v/>
       </c>
       <c r="B25" s="5"/>
@@ -1706,7 +1721,7 @@
     </row>
     <row r="26" customHeight="1" spans="1:8">
       <c r="A26" s="12" t="str">
-        <f>IF(G26&lt;&gt;"",UPPER(LEFT(G26,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G26,G26),"0000"),"")</f>
+        <f>IF(G26&lt;&gt;"",UPPER(LEFT(G26,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G26,G26),"0000"),"")</f>
         <v/>
       </c>
       <c r="B26" s="5"/>
@@ -1719,7 +1734,7 @@
     </row>
     <row r="27" customHeight="1" spans="1:8">
       <c r="A27" s="12" t="str">
-        <f>IF(G27&lt;&gt;"",UPPER(LEFT(G27,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G27,G27),"0000"),"")</f>
+        <f>IF(G27&lt;&gt;"",UPPER(LEFT(G27,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G27,G27),"0000"),"")</f>
         <v/>
       </c>
       <c r="B27" s="5"/>
@@ -1732,7 +1747,7 @@
     </row>
     <row r="28" customHeight="1" spans="1:8">
       <c r="A28" s="12" t="str">
-        <f>IF(G28&lt;&gt;"",UPPER(LEFT(G28,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G28,G28),"0000"),"")</f>
+        <f>IF(G28&lt;&gt;"",UPPER(LEFT(G28,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G28,G28),"0000"),"")</f>
         <v/>
       </c>
       <c r="B28" s="5"/>
@@ -1745,7 +1760,7 @@
     </row>
     <row r="29" customHeight="1" spans="1:8">
       <c r="A29" s="12" t="str">
-        <f>IF(G29&lt;&gt;"",UPPER(LEFT(G29,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G29,G29),"0000"),"")</f>
+        <f>IF(G29&lt;&gt;"",UPPER(LEFT(G29,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G29,G29),"0000"),"")</f>
         <v/>
       </c>
       <c r="B29" s="5"/>
@@ -1758,7 +1773,7 @@
     </row>
     <row r="30" customHeight="1" spans="1:8">
       <c r="A30" s="12" t="str">
-        <f>IF(G30&lt;&gt;"",UPPER(LEFT(G30,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G30,G30),"0000"),"")</f>
+        <f>IF(G30&lt;&gt;"",UPPER(LEFT(G30,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G30,G30),"0000"),"")</f>
         <v/>
       </c>
       <c r="B30" s="5"/>
@@ -1771,7 +1786,7 @@
     </row>
     <row r="31" customHeight="1" spans="1:8">
       <c r="A31" s="12" t="str">
-        <f>IF(G31&lt;&gt;"",UPPER(LEFT(G31,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G31,G31),"0000"),"")</f>
+        <f>IF(G31&lt;&gt;"",UPPER(LEFT(G31,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G31,G31),"0000"),"")</f>
         <v/>
       </c>
       <c r="B31" s="5"/>
@@ -1784,7 +1799,7 @@
     </row>
     <row r="32" customHeight="1" spans="1:8">
       <c r="A32" s="12" t="str">
-        <f>IF(G32&lt;&gt;"",UPPER(LEFT(G32,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G32,G32),"0000"),"")</f>
+        <f>IF(G32&lt;&gt;"",UPPER(LEFT(G32,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G32,G32),"0000"),"")</f>
         <v/>
       </c>
       <c r="B32" s="5"/>
@@ -1797,7 +1812,7 @@
     </row>
     <row r="33" customHeight="1" spans="1:8">
       <c r="A33" s="12" t="str">
-        <f>IF(G33&lt;&gt;"",UPPER(LEFT(G33,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G33,G33),"0000"),"")</f>
+        <f>IF(G33&lt;&gt;"",UPPER(LEFT(G33,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G33,G33),"0000"),"")</f>
         <v/>
       </c>
       <c r="B33" s="5"/>
@@ -1810,7 +1825,7 @@
     </row>
     <row r="34" customHeight="1" spans="1:8">
       <c r="A34" s="12" t="str">
-        <f>IF(G34&lt;&gt;"",UPPER(LEFT(G34,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G34,G34),"0000"),"")</f>
+        <f>IF(G34&lt;&gt;"",UPPER(LEFT(G34,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G34,G34),"0000"),"")</f>
         <v/>
       </c>
       <c r="B34" s="5"/>
@@ -1823,7 +1838,7 @@
     </row>
     <row r="35" customHeight="1" spans="1:8">
       <c r="A35" s="12" t="str">
-        <f>IF(G35&lt;&gt;"",UPPER(LEFT(G35,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G35,G35),"0000"),"")</f>
+        <f>IF(G35&lt;&gt;"",UPPER(LEFT(G35,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G35,G35),"0000"),"")</f>
         <v/>
       </c>
       <c r="B35" s="5"/>
@@ -1836,7 +1851,7 @@
     </row>
     <row r="36" customHeight="1" spans="1:8">
       <c r="A36" s="12" t="str">
-        <f>IF(G36&lt;&gt;"",UPPER(LEFT(G36,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G36,G36),"0000"),"")</f>
+        <f>IF(G36&lt;&gt;"",UPPER(LEFT(G36,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G36,G36),"0000"),"")</f>
         <v/>
       </c>
       <c r="B36" s="5"/>
@@ -1849,7 +1864,7 @@
     </row>
     <row r="37" customHeight="1" spans="1:8">
       <c r="A37" s="12" t="str">
-        <f>IF(G37&lt;&gt;"",UPPER(LEFT(G37,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G37,G37),"0000"),"")</f>
+        <f>IF(G37&lt;&gt;"",UPPER(LEFT(G37,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G37,G37),"0000"),"")</f>
         <v/>
       </c>
       <c r="B37" s="5"/>
@@ -1862,7 +1877,7 @@
     </row>
     <row r="38" customHeight="1" spans="1:8">
       <c r="A38" s="12" t="str">
-        <f>IF(G38&lt;&gt;"",UPPER(LEFT(G38,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G38,G38),"0000"),"")</f>
+        <f>IF(G38&lt;&gt;"",UPPER(LEFT(G38,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G38,G38),"0000"),"")</f>
         <v/>
       </c>
       <c r="B38" s="5"/>
@@ -1875,7 +1890,7 @@
     </row>
     <row r="39" customHeight="1" spans="1:8">
       <c r="A39" s="12" t="str">
-        <f>IF(G39&lt;&gt;"",UPPER(LEFT(G39,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G39,G39),"0000"),"")</f>
+        <f>IF(G39&lt;&gt;"",UPPER(LEFT(G39,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G39,G39),"0000"),"")</f>
         <v/>
       </c>
       <c r="B39" s="5"/>
@@ -1888,7 +1903,7 @@
     </row>
     <row r="40" customHeight="1" spans="1:8">
       <c r="A40" s="12" t="str">
-        <f>IF(G40&lt;&gt;"",UPPER(LEFT(G40,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G40,G40),"0000"),"")</f>
+        <f>IF(G40&lt;&gt;"",UPPER(LEFT(G40,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G40,G40),"0000"),"")</f>
         <v/>
       </c>
       <c r="B40" s="5"/>
@@ -1901,7 +1916,7 @@
     </row>
     <row r="41" customHeight="1" spans="1:8">
       <c r="A41" s="12" t="str">
-        <f>IF(G41&lt;&gt;"",UPPER(LEFT(G41,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G41,G41),"0000"),"")</f>
+        <f>IF(G41&lt;&gt;"",UPPER(LEFT(G41,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G41,G41),"0000"),"")</f>
         <v/>
       </c>
       <c r="B41" s="5"/>
@@ -1914,7 +1929,7 @@
     </row>
     <row r="42" customHeight="1" spans="1:8">
       <c r="A42" s="12" t="str">
-        <f>IF(G42&lt;&gt;"",UPPER(LEFT(G42,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G42,G42),"0000"),"")</f>
+        <f>IF(G42&lt;&gt;"",UPPER(LEFT(G42,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G42,G42),"0000"),"")</f>
         <v/>
       </c>
       <c r="B42" s="5"/>
@@ -1927,7 +1942,7 @@
     </row>
     <row r="43" customHeight="1" spans="1:8">
       <c r="A43" s="12" t="str">
-        <f>IF(G43&lt;&gt;"",UPPER(LEFT(G43,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G43,G43),"0000"),"")</f>
+        <f>IF(G43&lt;&gt;"",UPPER(LEFT(G43,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G43,G43),"0000"),"")</f>
         <v/>
       </c>
       <c r="B43" s="5"/>
@@ -1940,7 +1955,7 @@
     </row>
     <row r="44" customHeight="1" spans="1:8">
       <c r="A44" s="12" t="str">
-        <f>IF(G44&lt;&gt;"",UPPER(LEFT(G44,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G44,G44),"0000"),"")</f>
+        <f>IF(G44&lt;&gt;"",UPPER(LEFT(G44,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G44,G44),"0000"),"")</f>
         <v/>
       </c>
       <c r="B44" s="5"/>
@@ -1953,7 +1968,7 @@
     </row>
     <row r="45" customHeight="1" spans="1:8">
       <c r="A45" s="12" t="str">
-        <f>IF(G45&lt;&gt;"",UPPER(LEFT(G45,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G45,G45),"0000"),"")</f>
+        <f>IF(G45&lt;&gt;"",UPPER(LEFT(G45,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G45,G45),"0000"),"")</f>
         <v/>
       </c>
       <c r="B45" s="5"/>
@@ -1966,7 +1981,7 @@
     </row>
     <row r="46" customHeight="1" spans="1:8">
       <c r="A46" s="12" t="str">
-        <f>IF(G46&lt;&gt;"",UPPER(LEFT(G46,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G46,G46),"0000"),"")</f>
+        <f>IF(G46&lt;&gt;"",UPPER(LEFT(G46,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G46,G46),"0000"),"")</f>
         <v/>
       </c>
       <c r="B46" s="5"/>
@@ -1979,7 +1994,7 @@
     </row>
     <row r="47" customHeight="1" spans="1:8">
       <c r="A47" s="12" t="str">
-        <f>IF(G47&lt;&gt;"",UPPER(LEFT(G47,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G47,G47),"0000"),"")</f>
+        <f>IF(G47&lt;&gt;"",UPPER(LEFT(G47,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G47,G47),"0000"),"")</f>
         <v/>
       </c>
       <c r="B47" s="5"/>
@@ -1992,7 +2007,7 @@
     </row>
     <row r="48" customHeight="1" spans="1:8">
       <c r="A48" s="12" t="str">
-        <f>IF(G48&lt;&gt;"",UPPER(LEFT(G48,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G48,G48),"0000"),"")</f>
+        <f>IF(G48&lt;&gt;"",UPPER(LEFT(G48,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G48,G48),"0000"),"")</f>
         <v/>
       </c>
       <c r="B48" s="5"/>
@@ -2005,7 +2020,7 @@
     </row>
     <row r="49" customHeight="1" spans="1:8">
       <c r="A49" s="12" t="str">
-        <f>IF(G49&lt;&gt;"",UPPER(LEFT(G49,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G49,G49),"0000"),"")</f>
+        <f>IF(G49&lt;&gt;"",UPPER(LEFT(G49,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G49,G49),"0000"),"")</f>
         <v/>
       </c>
       <c r="B49" s="5"/>
@@ -2018,7 +2033,7 @@
     </row>
     <row r="50" customHeight="1" spans="1:8">
       <c r="A50" s="12" t="str">
-        <f>IF(G50&lt;&gt;"",UPPER(LEFT(G50,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G50,G50),"0000"),"")</f>
+        <f>IF(G50&lt;&gt;"",UPPER(LEFT(G50,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G50,G50),"0000"),"")</f>
         <v/>
       </c>
       <c r="B50" s="5"/>
@@ -2031,7 +2046,7 @@
     </row>
     <row r="51" customHeight="1" spans="1:8">
       <c r="A51" s="12" t="str">
-        <f>IF(G51&lt;&gt;"",UPPER(LEFT(G51,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G51,G51),"0000"),"")</f>
+        <f>IF(G51&lt;&gt;"",UPPER(LEFT(G51,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G51,G51),"0000"),"")</f>
         <v/>
       </c>
       <c r="B51" s="5"/>
@@ -2044,7 +2059,7 @@
     </row>
     <row r="52" customHeight="1" spans="1:8">
       <c r="A52" s="12" t="str">
-        <f>IF(G52&lt;&gt;"",UPPER(LEFT(G52,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G52,G52),"0000"),"")</f>
+        <f>IF(G52&lt;&gt;"",UPPER(LEFT(G52,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G52,G52),"0000"),"")</f>
         <v/>
       </c>
       <c r="B52" s="5"/>
@@ -2057,7 +2072,7 @@
     </row>
     <row r="53" customHeight="1" spans="1:8">
       <c r="A53" s="12" t="str">
-        <f>IF(G53&lt;&gt;"",UPPER(LEFT(G53,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G53,G53),"0000"),"")</f>
+        <f>IF(G53&lt;&gt;"",UPPER(LEFT(G53,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G53,G53),"0000"),"")</f>
         <v/>
       </c>
       <c r="B53" s="5"/>
@@ -2070,7 +2085,7 @@
     </row>
     <row r="54" customHeight="1" spans="1:8">
       <c r="A54" s="12" t="str">
-        <f>IF(G54&lt;&gt;"",UPPER(LEFT(G54,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G54,G54),"0000"),"")</f>
+        <f>IF(G54&lt;&gt;"",UPPER(LEFT(G54,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G54,G54),"0000"),"")</f>
         <v/>
       </c>
       <c r="B54" s="5"/>
@@ -2083,7 +2098,7 @@
     </row>
     <row r="55" customHeight="1" spans="1:8">
       <c r="A55" s="12" t="str">
-        <f>IF(G55&lt;&gt;"",UPPER(LEFT(G55,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G55,G55),"0000"),"")</f>
+        <f>IF(G55&lt;&gt;"",UPPER(LEFT(G55,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G55,G55),"0000"),"")</f>
         <v/>
       </c>
       <c r="B55" s="5"/>
@@ -2096,7 +2111,7 @@
     </row>
     <row r="56" customHeight="1" spans="1:8">
       <c r="A56" s="12" t="str">
-        <f>IF(G56&lt;&gt;"",UPPER(LEFT(G56,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G56,G56),"0000"),"")</f>
+        <f>IF(G56&lt;&gt;"",UPPER(LEFT(G56,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G56,G56),"0000"),"")</f>
         <v/>
       </c>
       <c r="B56" s="5"/>
@@ -2109,7 +2124,7 @@
     </row>
     <row r="57" customHeight="1" spans="1:8">
       <c r="A57" s="12" t="str">
-        <f>IF(G57&lt;&gt;"",UPPER(LEFT(G57,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G57,G57),"0000"),"")</f>
+        <f>IF(G57&lt;&gt;"",UPPER(LEFT(G57,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G57,G57),"0000"),"")</f>
         <v/>
       </c>
       <c r="B57" s="5"/>
@@ -2122,7 +2137,7 @@
     </row>
     <row r="58" customHeight="1" spans="1:8">
       <c r="A58" s="12" t="str">
-        <f>IF(G58&lt;&gt;"",UPPER(LEFT(G58,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G58,G58),"0000"),"")</f>
+        <f>IF(G58&lt;&gt;"",UPPER(LEFT(G58,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G58,G58),"0000"),"")</f>
         <v/>
       </c>
       <c r="B58" s="5"/>
@@ -2135,7 +2150,7 @@
     </row>
     <row r="59" customHeight="1" spans="1:8">
       <c r="A59" s="12" t="str">
-        <f>IF(G59&lt;&gt;"",UPPER(LEFT(G59,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G59,G59),"0000"),"")</f>
+        <f>IF(G59&lt;&gt;"",UPPER(LEFT(G59,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G59,G59),"0000"),"")</f>
         <v/>
       </c>
       <c r="B59" s="5"/>
@@ -2148,7 +2163,7 @@
     </row>
     <row r="60" customHeight="1" spans="1:8">
       <c r="A60" s="12" t="str">
-        <f>IF(G60&lt;&gt;"",UPPER(LEFT(G60,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G60,G60),"0000"),"")</f>
+        <f>IF(G60&lt;&gt;"",UPPER(LEFT(G60,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G60,G60),"0000"),"")</f>
         <v/>
       </c>
       <c r="B60" s="5"/>
@@ -2161,7 +2176,7 @@
     </row>
     <row r="61" customHeight="1" spans="1:8">
       <c r="A61" s="12" t="str">
-        <f>IF(G61&lt;&gt;"",UPPER(LEFT(G61,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G61,G61),"0000"),"")</f>
+        <f>IF(G61&lt;&gt;"",UPPER(LEFT(G61,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G61,G61),"0000"),"")</f>
         <v/>
       </c>
       <c r="B61" s="5"/>
@@ -2174,7 +2189,7 @@
     </row>
     <row r="62" customHeight="1" spans="1:8">
       <c r="A62" s="12" t="str">
-        <f>IF(G62&lt;&gt;"",UPPER(LEFT(G62,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G62,G62),"0000"),"")</f>
+        <f>IF(G62&lt;&gt;"",UPPER(LEFT(G62,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G62,G62),"0000"),"")</f>
         <v/>
       </c>
       <c r="B62" s="5"/>
@@ -2187,7 +2202,7 @@
     </row>
     <row r="63" customHeight="1" spans="1:8">
       <c r="A63" s="12" t="str">
-        <f>IF(G63&lt;&gt;"",UPPER(LEFT(G63,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G63,G63),"0000"),"")</f>
+        <f>IF(G63&lt;&gt;"",UPPER(LEFT(G63,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G63,G63),"0000"),"")</f>
         <v/>
       </c>
       <c r="B63" s="5"/>
@@ -2200,7 +2215,7 @@
     </row>
     <row r="64" customHeight="1" spans="1:8">
       <c r="A64" s="12" t="str">
-        <f>IF(G64&lt;&gt;"",UPPER(LEFT(G64,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G64,G64),"0000"),"")</f>
+        <f>IF(G64&lt;&gt;"",UPPER(LEFT(G64,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G64,G64),"0000"),"")</f>
         <v/>
       </c>
       <c r="B64" s="5"/>
@@ -2213,7 +2228,7 @@
     </row>
     <row r="65" customHeight="1" spans="1:8">
       <c r="A65" s="12" t="str">
-        <f>IF(G65&lt;&gt;"",UPPER(LEFT(G65,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G65,G65),"0000"),"")</f>
+        <f>IF(G65&lt;&gt;"",UPPER(LEFT(G65,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G65,G65),"0000"),"")</f>
         <v/>
       </c>
       <c r="B65" s="5"/>
@@ -2226,7 +2241,7 @@
     </row>
     <row r="66" customHeight="1" spans="1:8">
       <c r="A66" s="12" t="str">
-        <f>IF(G66&lt;&gt;"",UPPER(LEFT(G66,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G66,G66),"0000"),"")</f>
+        <f>IF(G66&lt;&gt;"",UPPER(LEFT(G66,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G66,G66),"0000"),"")</f>
         <v/>
       </c>
       <c r="B66" s="5"/>
@@ -2239,7 +2254,7 @@
     </row>
     <row r="67" customHeight="1" spans="1:8">
       <c r="A67" s="12" t="str">
-        <f>IF(G67&lt;&gt;"",UPPER(LEFT(G67,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G67,G67),"0000"),"")</f>
+        <f>IF(G67&lt;&gt;"",UPPER(LEFT(G67,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G67,G67),"0000"),"")</f>
         <v/>
       </c>
       <c r="B67" s="5"/>
@@ -2252,7 +2267,7 @@
     </row>
     <row r="68" customHeight="1" spans="1:8">
       <c r="A68" s="12" t="str">
-        <f>IF(G68&lt;&gt;"",UPPER(LEFT(G68,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G68,G68),"0000"),"")</f>
+        <f>IF(G68&lt;&gt;"",UPPER(LEFT(G68,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G68,G68),"0000"),"")</f>
         <v/>
       </c>
       <c r="B68" s="5"/>
@@ -2265,7 +2280,7 @@
     </row>
     <row r="69" customHeight="1" spans="1:8">
       <c r="A69" s="12" t="str">
-        <f>IF(G69&lt;&gt;"",UPPER(LEFT(G69,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G69,G69),"0000"),"")</f>
+        <f>IF(G69&lt;&gt;"",UPPER(LEFT(G69,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G69,G69),"0000"),"")</f>
         <v/>
       </c>
       <c r="B69" s="5"/>
@@ -2278,7 +2293,7 @@
     </row>
     <row r="70" customHeight="1" spans="1:8">
       <c r="A70" s="12" t="str">
-        <f>IF(G70&lt;&gt;"",UPPER(LEFT(G70,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G70,G70),"0000"),"")</f>
+        <f>IF(G70&lt;&gt;"",UPPER(LEFT(G70,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G70,G70),"0000"),"")</f>
         <v/>
       </c>
       <c r="B70" s="5"/>
@@ -2291,7 +2306,7 @@
     </row>
     <row r="71" customHeight="1" spans="1:8">
       <c r="A71" s="12" t="str">
-        <f>IF(G71&lt;&gt;"",UPPER(LEFT(G71,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G71,G71),"0000"),"")</f>
+        <f>IF(G71&lt;&gt;"",UPPER(LEFT(G71,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G71,G71),"0000"),"")</f>
         <v/>
       </c>
       <c r="B71" s="5"/>
@@ -2304,7 +2319,7 @@
     </row>
     <row r="72" customHeight="1" spans="1:8">
       <c r="A72" s="12" t="str">
-        <f>IF(G72&lt;&gt;"",UPPER(LEFT(G72,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G72,G72),"0000"),"")</f>
+        <f>IF(G72&lt;&gt;"",UPPER(LEFT(G72,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G72,G72),"0000"),"")</f>
         <v/>
       </c>
       <c r="B72" s="5"/>
@@ -2317,7 +2332,7 @@
     </row>
     <row r="73" customHeight="1" spans="1:8">
       <c r="A73" s="12" t="str">
-        <f>IF(G73&lt;&gt;"",UPPER(LEFT(G73,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G73,G73),"0000"),"")</f>
+        <f>IF(G73&lt;&gt;"",UPPER(LEFT(G73,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G73,G73),"0000"),"")</f>
         <v/>
       </c>
       <c r="B73" s="5"/>
@@ -2330,7 +2345,7 @@
     </row>
     <row r="74" customHeight="1" spans="1:8">
       <c r="A74" s="12" t="str">
-        <f>IF(G74&lt;&gt;"",UPPER(LEFT(G74,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G74,G74),"0000"),"")</f>
+        <f>IF(G74&lt;&gt;"",UPPER(LEFT(G74,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G74,G74),"0000"),"")</f>
         <v/>
       </c>
       <c r="B74" s="5"/>
@@ -2343,7 +2358,7 @@
     </row>
     <row r="75" customHeight="1" spans="1:8">
       <c r="A75" s="12" t="str">
-        <f>IF(G75&lt;&gt;"",UPPER(LEFT(G75,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G75,G75),"0000"),"")</f>
+        <f>IF(G75&lt;&gt;"",UPPER(LEFT(G75,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G75,G75),"0000"),"")</f>
         <v/>
       </c>
       <c r="B75" s="5"/>
@@ -2356,7 +2371,7 @@
     </row>
     <row r="76" customHeight="1" spans="1:8">
       <c r="A76" s="12" t="str">
-        <f>IF(G76&lt;&gt;"",UPPER(LEFT(G76,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G76,G76),"0000"),"")</f>
+        <f>IF(G76&lt;&gt;"",UPPER(LEFT(G76,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G76,G76),"0000"),"")</f>
         <v/>
       </c>
       <c r="B76" s="5"/>
@@ -2369,7 +2384,7 @@
     </row>
     <row r="77" customHeight="1" spans="1:8">
       <c r="A77" s="12" t="str">
-        <f>IF(G77&lt;&gt;"",UPPER(LEFT(G77,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G77,G77),"0000"),"")</f>
+        <f>IF(G77&lt;&gt;"",UPPER(LEFT(G77,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G77,G77),"0000"),"")</f>
         <v/>
       </c>
       <c r="B77" s="5"/>
@@ -2382,7 +2397,7 @@
     </row>
     <row r="78" customHeight="1" spans="1:8">
       <c r="A78" s="12" t="str">
-        <f>IF(G78&lt;&gt;"",UPPER(LEFT(G78,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G78,G78),"0000"),"")</f>
+        <f>IF(G78&lt;&gt;"",UPPER(LEFT(G78,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G78,G78),"0000"),"")</f>
         <v/>
       </c>
       <c r="B78" s="5"/>
@@ -2395,7 +2410,7 @@
     </row>
     <row r="79" customHeight="1" spans="1:8">
       <c r="A79" s="12" t="str">
-        <f>IF(G79&lt;&gt;"",UPPER(LEFT(G79,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G79,G79),"0000"),"")</f>
+        <f>IF(G79&lt;&gt;"",UPPER(LEFT(G79,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G79,G79),"0000"),"")</f>
         <v/>
       </c>
       <c r="B79" s="5"/>
@@ -2408,7 +2423,7 @@
     </row>
     <row r="80" customHeight="1" spans="1:8">
       <c r="A80" s="12" t="str">
-        <f>IF(G80&lt;&gt;"",UPPER(LEFT(G80,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G80,G80),"0000"),"")</f>
+        <f>IF(G80&lt;&gt;"",UPPER(LEFT(G80,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G80,G80),"0000"),"")</f>
         <v/>
       </c>
       <c r="B80" s="5"/>
@@ -2421,7 +2436,7 @@
     </row>
     <row r="81" customHeight="1" spans="1:8">
       <c r="A81" s="12" t="str">
-        <f>IF(G81&lt;&gt;"",UPPER(LEFT(G81,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G81,G81),"0000"),"")</f>
+        <f>IF(G81&lt;&gt;"",UPPER(LEFT(G81,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G81,G81),"0000"),"")</f>
         <v/>
       </c>
       <c r="B81" s="5"/>
@@ -2434,7 +2449,7 @@
     </row>
     <row r="82" customHeight="1" spans="1:8">
       <c r="A82" s="12" t="str">
-        <f>IF(G82&lt;&gt;"",UPPER(LEFT(G82,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G82,G82),"0000"),"")</f>
+        <f>IF(G82&lt;&gt;"",UPPER(LEFT(G82,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G82,G82),"0000"),"")</f>
         <v/>
       </c>
       <c r="B82" s="5"/>
@@ -2447,7 +2462,7 @@
     </row>
     <row r="83" customHeight="1" spans="1:8">
       <c r="A83" s="12" t="str">
-        <f>IF(G83&lt;&gt;"",UPPER(LEFT(G83,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G83,G83),"0000"),"")</f>
+        <f>IF(G83&lt;&gt;"",UPPER(LEFT(G83,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G83,G83),"0000"),"")</f>
         <v/>
       </c>
       <c r="B83" s="5"/>
@@ -2460,7 +2475,7 @@
     </row>
     <row r="84" customHeight="1" spans="1:8">
       <c r="A84" s="12" t="str">
-        <f>IF(G84&lt;&gt;"",UPPER(LEFT(G84,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G84,G84),"0000"),"")</f>
+        <f>IF(G84&lt;&gt;"",UPPER(LEFT(G84,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G84,G84),"0000"),"")</f>
         <v/>
       </c>
       <c r="B84" s="5"/>
@@ -2473,7 +2488,7 @@
     </row>
     <row r="85" customHeight="1" spans="1:8">
       <c r="A85" s="12" t="str">
-        <f>IF(G85&lt;&gt;"",UPPER(LEFT(G85,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G85,G85),"0000"),"")</f>
+        <f>IF(G85&lt;&gt;"",UPPER(LEFT(G85,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G85,G85),"0000"),"")</f>
         <v/>
       </c>
       <c r="B85" s="5"/>
@@ -2486,7 +2501,7 @@
     </row>
     <row r="86" customHeight="1" spans="1:8">
       <c r="A86" s="12" t="str">
-        <f>IF(G86&lt;&gt;"",UPPER(LEFT(G86,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G86,G86),"0000"),"")</f>
+        <f>IF(G86&lt;&gt;"",UPPER(LEFT(G86,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G86,G86),"0000"),"")</f>
         <v/>
       </c>
       <c r="B86" s="5"/>
@@ -2499,7 +2514,7 @@
     </row>
     <row r="87" customHeight="1" spans="1:8">
       <c r="A87" s="12" t="str">
-        <f>IF(G87&lt;&gt;"",UPPER(LEFT(G87,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G87,G87),"0000"),"")</f>
+        <f>IF(G87&lt;&gt;"",UPPER(LEFT(G87,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G87,G87),"0000"),"")</f>
         <v/>
       </c>
       <c r="B87" s="5"/>
@@ -2512,7 +2527,7 @@
     </row>
     <row r="88" customHeight="1" spans="1:8">
       <c r="A88" s="12" t="str">
-        <f>IF(G88&lt;&gt;"",UPPER(LEFT(G88,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G88,G88),"0000"),"")</f>
+        <f>IF(G88&lt;&gt;"",UPPER(LEFT(G88,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G88,G88),"0000"),"")</f>
         <v/>
       </c>
       <c r="B88" s="5"/>
@@ -2525,7 +2540,7 @@
     </row>
     <row r="89" customHeight="1" spans="1:8">
       <c r="A89" s="12" t="str">
-        <f>IF(G89&lt;&gt;"",UPPER(LEFT(G89,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G89,G89),"0000"),"")</f>
+        <f>IF(G89&lt;&gt;"",UPPER(LEFT(G89,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G89,G89),"0000"),"")</f>
         <v/>
       </c>
       <c r="B89" s="5"/>
@@ -2538,7 +2553,7 @@
     </row>
     <row r="90" customHeight="1" spans="1:8">
       <c r="A90" s="12" t="str">
-        <f>IF(G90&lt;&gt;"",UPPER(LEFT(G90,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G90,G90),"0000"),"")</f>
+        <f>IF(G90&lt;&gt;"",UPPER(LEFT(G90,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G90,G90),"0000"),"")</f>
         <v/>
       </c>
       <c r="B90" s="5"/>
@@ -2551,7 +2566,7 @@
     </row>
     <row r="91" customHeight="1" spans="1:8">
       <c r="A91" s="12" t="str">
-        <f>IF(G91&lt;&gt;"",UPPER(LEFT(G91,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G91,G91),"0000"),"")</f>
+        <f>IF(G91&lt;&gt;"",UPPER(LEFT(G91,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G91,G91),"0000"),"")</f>
         <v/>
       </c>
       <c r="B91" s="5"/>
@@ -2564,7 +2579,7 @@
     </row>
     <row r="92" customHeight="1" spans="1:8">
       <c r="A92" s="12" t="str">
-        <f>IF(G92&lt;&gt;"",UPPER(LEFT(G92,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G92,G92),"0000"),"")</f>
+        <f>IF(G92&lt;&gt;"",UPPER(LEFT(G92,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G92,G92),"0000"),"")</f>
         <v/>
       </c>
       <c r="B92" s="5"/>
@@ -2577,7 +2592,7 @@
     </row>
     <row r="93" customHeight="1" spans="1:8">
       <c r="A93" s="12" t="str">
-        <f>IF(G93&lt;&gt;"",UPPER(LEFT(G93,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G93,G93),"0000"),"")</f>
+        <f>IF(G93&lt;&gt;"",UPPER(LEFT(G93,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G93,G93),"0000"),"")</f>
         <v/>
       </c>
       <c r="B93" s="5"/>
@@ -2590,7 +2605,7 @@
     </row>
     <row r="94" customHeight="1" spans="1:8">
       <c r="A94" s="12" t="str">
-        <f>IF(G94&lt;&gt;"",UPPER(LEFT(G94,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G94,G94),"0000"),"")</f>
+        <f>IF(G94&lt;&gt;"",UPPER(LEFT(G94,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G94,G94),"0000"),"")</f>
         <v/>
       </c>
       <c r="B94" s="5"/>
@@ -2603,7 +2618,7 @@
     </row>
     <row r="95" customHeight="1" spans="1:8">
       <c r="A95" s="12" t="str">
-        <f>IF(G95&lt;&gt;"",UPPER(LEFT(G95,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G95,G95),"0000"),"")</f>
+        <f>IF(G95&lt;&gt;"",UPPER(LEFT(G95,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G95,G95),"0000"),"")</f>
         <v/>
       </c>
       <c r="B95" s="5"/>
@@ -2616,7 +2631,7 @@
     </row>
     <row r="96" customHeight="1" spans="1:8">
       <c r="A96" s="12" t="str">
-        <f>IF(G96&lt;&gt;"",UPPER(LEFT(G96,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G96,G96),"0000"),"")</f>
+        <f>IF(G96&lt;&gt;"",UPPER(LEFT(G96,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G96,G96),"0000"),"")</f>
         <v/>
       </c>
       <c r="B96" s="5"/>
@@ -2629,7 +2644,7 @@
     </row>
     <row r="97" customHeight="1" spans="1:8">
       <c r="A97" s="12" t="str">
-        <f>IF(G97&lt;&gt;"",UPPER(LEFT(G97,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G97,G97),"0000"),"")</f>
+        <f>IF(G97&lt;&gt;"",UPPER(LEFT(G97,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G97,G97),"0000"),"")</f>
         <v/>
       </c>
       <c r="B97" s="5"/>
@@ -2642,7 +2657,7 @@
     </row>
     <row r="98" customHeight="1" spans="1:8">
       <c r="A98" s="12" t="str">
-        <f>IF(G98&lt;&gt;"",UPPER(LEFT(G98,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G98,G98),"0000"),"")</f>
+        <f>IF(G98&lt;&gt;"",UPPER(LEFT(G98,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G98,G98),"0000"),"")</f>
         <v/>
       </c>
       <c r="B98" s="5"/>
@@ -2655,7 +2670,7 @@
     </row>
     <row r="99" customHeight="1" spans="1:8">
       <c r="A99" s="12" t="str">
-        <f>IF(G99&lt;&gt;"",UPPER(LEFT(G99,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G99,G99),"0000"),"")</f>
+        <f>IF(G99&lt;&gt;"",UPPER(LEFT(G99,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G99,G99),"0000"),"")</f>
         <v/>
       </c>
       <c r="B99" s="5"/>
@@ -2668,7 +2683,7 @@
     </row>
     <row r="100" customHeight="1" spans="1:8">
       <c r="A100" s="12" t="str">
-        <f>IF(G100&lt;&gt;"",UPPER(LEFT(G100,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G100,G100),"0000"),"")</f>
+        <f>IF(G100&lt;&gt;"",UPPER(LEFT(G100,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G100,G100),"0000"),"")</f>
         <v/>
       </c>
       <c r="B100" s="5"/>
@@ -2681,7 +2696,7 @@
     </row>
     <row r="101" customHeight="1" spans="1:8">
       <c r="A101" s="12" t="str">
-        <f>IF(G101&lt;&gt;"",UPPER(LEFT(G101,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G101,G101),"0000"),"")</f>
+        <f>IF(G101&lt;&gt;"",UPPER(LEFT(G101,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G101,G101),"0000"),"")</f>
         <v/>
       </c>
       <c r="B101" s="5"/>
@@ -2694,7 +2709,7 @@
     </row>
     <row r="102" customHeight="1" spans="1:8">
       <c r="A102" s="12" t="str">
-        <f>IF(G102&lt;&gt;"",UPPER(LEFT(G102,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G102,G102),"0000"),"")</f>
+        <f>IF(G102&lt;&gt;"",UPPER(LEFT(G102,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G102,G102),"0000"),"")</f>
         <v/>
       </c>
       <c r="B102" s="5"/>
@@ -2707,7 +2722,7 @@
     </row>
     <row r="103" customHeight="1" spans="1:8">
       <c r="A103" s="12" t="str">
-        <f>IF(G103&lt;&gt;"",UPPER(LEFT(G103,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G103,G103),"0000"),"")</f>
+        <f>IF(G103&lt;&gt;"",UPPER(LEFT(G103,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G103,G103),"0000"),"")</f>
         <v/>
       </c>
       <c r="B103" s="5"/>
@@ -2720,7 +2735,7 @@
     </row>
     <row r="104" customHeight="1" spans="1:8">
       <c r="A104" s="12" t="str">
-        <f>IF(G104&lt;&gt;"",UPPER(LEFT(G104,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G104,G104),"0000"),"")</f>
+        <f>IF(G104&lt;&gt;"",UPPER(LEFT(G104,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G104,G104),"0000"),"")</f>
         <v/>
       </c>
       <c r="B104" s="5"/>
@@ -2733,7 +2748,7 @@
     </row>
     <row r="105" customHeight="1" spans="1:8">
       <c r="A105" s="12" t="str">
-        <f>IF(G105&lt;&gt;"",UPPER(LEFT(G105,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G105,G105),"0000"),"")</f>
+        <f>IF(G105&lt;&gt;"",UPPER(LEFT(G105,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G105,G105),"0000"),"")</f>
         <v/>
       </c>
       <c r="B105" s="5"/>
@@ -2746,7 +2761,7 @@
     </row>
     <row r="106" customHeight="1" spans="1:8">
       <c r="A106" s="12" t="str">
-        <f>IF(G106&lt;&gt;"",UPPER(LEFT(G106,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G106,G106),"0000"),"")</f>
+        <f>IF(G106&lt;&gt;"",UPPER(LEFT(G106,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G106,G106),"0000"),"")</f>
         <v/>
       </c>
       <c r="B106" s="5"/>
@@ -2759,7 +2774,7 @@
     </row>
     <row r="107" customHeight="1" spans="1:8">
       <c r="A107" s="12" t="str">
-        <f>IF(G107&lt;&gt;"",UPPER(LEFT(G107,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G107,G107),"0000"),"")</f>
+        <f>IF(G107&lt;&gt;"",UPPER(LEFT(G107,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G107,G107),"0000"),"")</f>
         <v/>
       </c>
       <c r="B107" s="5"/>
@@ -2772,7 +2787,7 @@
     </row>
     <row r="108" customHeight="1" spans="1:8">
       <c r="A108" s="12" t="str">
-        <f>IF(G108&lt;&gt;"",UPPER(LEFT(G108,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G108,G108),"0000"),"")</f>
+        <f>IF(G108&lt;&gt;"",UPPER(LEFT(G108,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G108,G108),"0000"),"")</f>
         <v/>
       </c>
       <c r="B108" s="5"/>
@@ -2785,7 +2800,7 @@
     </row>
     <row r="109" customHeight="1" spans="1:8">
       <c r="A109" s="12" t="str">
-        <f>IF(G109&lt;&gt;"",UPPER(LEFT(G109,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G109,G109),"0000"),"")</f>
+        <f>IF(G109&lt;&gt;"",UPPER(LEFT(G109,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G109,G109),"0000"),"")</f>
         <v/>
       </c>
       <c r="B109" s="5"/>
@@ -2798,7 +2813,7 @@
     </row>
     <row r="110" customHeight="1" spans="1:8">
       <c r="A110" s="12" t="str">
-        <f>IF(G110&lt;&gt;"",UPPER(LEFT(G110,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G110,G110),"0000"),"")</f>
+        <f>IF(G110&lt;&gt;"",UPPER(LEFT(G110,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G110,G110),"0000"),"")</f>
         <v/>
       </c>
       <c r="B110" s="5"/>
@@ -2811,7 +2826,7 @@
     </row>
     <row r="111" customHeight="1" spans="1:8">
       <c r="A111" s="12" t="str">
-        <f>IF(G111&lt;&gt;"",UPPER(LEFT(G111,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G111,G111),"0000"),"")</f>
+        <f>IF(G111&lt;&gt;"",UPPER(LEFT(G111,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G111,G111),"0000"),"")</f>
         <v/>
       </c>
       <c r="B111" s="5"/>
@@ -2824,7 +2839,7 @@
     </row>
     <row r="112" customHeight="1" spans="1:8">
       <c r="A112" s="12" t="str">
-        <f>IF(G112&lt;&gt;"",UPPER(LEFT(G112,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G112,G112),"0000"),"")</f>
+        <f>IF(G112&lt;&gt;"",UPPER(LEFT(G112,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G112,G112),"0000"),"")</f>
         <v/>
       </c>
       <c r="B112" s="5"/>
@@ -2837,7 +2852,7 @@
     </row>
     <row r="113" customHeight="1" spans="1:8">
       <c r="A113" s="12" t="str">
-        <f>IF(G113&lt;&gt;"",UPPER(LEFT(G113,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G113,G113),"0000"),"")</f>
+        <f>IF(G113&lt;&gt;"",UPPER(LEFT(G113,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G113,G113),"0000"),"")</f>
         <v/>
       </c>
       <c r="B113" s="5"/>
@@ -2850,7 +2865,7 @@
     </row>
     <row r="114" customHeight="1" spans="1:8">
       <c r="A114" s="12" t="str">
-        <f>IF(G114&lt;&gt;"",UPPER(LEFT(G114,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G114,G114),"0000"),"")</f>
+        <f>IF(G114&lt;&gt;"",UPPER(LEFT(G114,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G114,G114),"0000"),"")</f>
         <v/>
       </c>
       <c r="B114" s="5"/>
@@ -2863,7 +2878,7 @@
     </row>
     <row r="115" customHeight="1" spans="1:8">
       <c r="A115" s="12" t="str">
-        <f>IF(G115&lt;&gt;"",UPPER(LEFT(G115,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G115,G115),"0000"),"")</f>
+        <f>IF(G115&lt;&gt;"",UPPER(LEFT(G115,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G115,G115),"0000"),"")</f>
         <v/>
       </c>
       <c r="B115" s="5"/>
@@ -2876,7 +2891,7 @@
     </row>
     <row r="116" customHeight="1" spans="1:8">
       <c r="A116" s="12" t="str">
-        <f>IF(G116&lt;&gt;"",UPPER(LEFT(G116,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G116,G116),"0000"),"")</f>
+        <f>IF(G116&lt;&gt;"",UPPER(LEFT(G116,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G116,G116),"0000"),"")</f>
         <v/>
       </c>
       <c r="B116" s="5"/>
@@ -2889,7 +2904,7 @@
     </row>
     <row r="117" customHeight="1" spans="1:8">
       <c r="A117" s="12" t="str">
-        <f>IF(G117&lt;&gt;"",UPPER(LEFT(G117,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G117,G117),"0000"),"")</f>
+        <f>IF(G117&lt;&gt;"",UPPER(LEFT(G117,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G117,G117),"0000"),"")</f>
         <v/>
       </c>
       <c r="B117" s="5"/>
@@ -2902,7 +2917,7 @@
     </row>
     <row r="118" customHeight="1" spans="1:8">
       <c r="A118" s="12" t="str">
-        <f>IF(G118&lt;&gt;"",UPPER(LEFT(G118,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G118,G118),"0000"),"")</f>
+        <f>IF(G118&lt;&gt;"",UPPER(LEFT(G118,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G118,G118),"0000"),"")</f>
         <v/>
       </c>
       <c r="B118" s="5"/>
@@ -2915,7 +2930,7 @@
     </row>
     <row r="119" customHeight="1" spans="1:8">
       <c r="A119" s="12" t="str">
-        <f>IF(G119&lt;&gt;"",UPPER(LEFT(G119,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G119,G119),"0000"),"")</f>
+        <f>IF(G119&lt;&gt;"",UPPER(LEFT(G119,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G119,G119),"0000"),"")</f>
         <v/>
       </c>
       <c r="B119" s="5"/>
@@ -2928,7 +2943,7 @@
     </row>
     <row r="120" customHeight="1" spans="1:8">
       <c r="A120" s="12" t="str">
-        <f>IF(G120&lt;&gt;"",UPPER(LEFT(G120,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G120,G120),"0000"),"")</f>
+        <f>IF(G120&lt;&gt;"",UPPER(LEFT(G120,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G120,G120),"0000"),"")</f>
         <v/>
       </c>
       <c r="B120" s="5"/>
@@ -2941,7 +2956,7 @@
     </row>
     <row r="121" customHeight="1" spans="1:8">
       <c r="A121" s="12" t="str">
-        <f>IF(G121&lt;&gt;"",UPPER(LEFT(G121,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G121,G121),"0000"),"")</f>
+        <f>IF(G121&lt;&gt;"",UPPER(LEFT(G121,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G121,G121),"0000"),"")</f>
         <v/>
       </c>
       <c r="B121" s="5"/>
@@ -2954,7 +2969,7 @@
     </row>
     <row r="122" customHeight="1" spans="1:8">
       <c r="A122" s="12" t="str">
-        <f>IF(G122&lt;&gt;"",UPPER(LEFT(G122,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G122,G122),"0000"),"")</f>
+        <f>IF(G122&lt;&gt;"",UPPER(LEFT(G122,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G122,G122),"0000"),"")</f>
         <v/>
       </c>
       <c r="B122" s="5"/>
@@ -2967,7 +2982,7 @@
     </row>
     <row r="123" customHeight="1" spans="1:8">
       <c r="A123" s="12" t="str">
-        <f>IF(G123&lt;&gt;"",UPPER(LEFT(G123,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G123,G123),"0000"),"")</f>
+        <f>IF(G123&lt;&gt;"",UPPER(LEFT(G123,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G123,G123),"0000"),"")</f>
         <v/>
       </c>
       <c r="B123" s="5"/>
@@ -2980,7 +2995,7 @@
     </row>
     <row r="124" customHeight="1" spans="1:8">
       <c r="A124" s="12" t="str">
-        <f>IF(G124&lt;&gt;"",UPPER(LEFT(G124,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G124,G124),"0000"),"")</f>
+        <f>IF(G124&lt;&gt;"",UPPER(LEFT(G124,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G124,G124),"0000"),"")</f>
         <v/>
       </c>
       <c r="B124" s="5"/>
@@ -2993,7 +3008,7 @@
     </row>
     <row r="125" customHeight="1" spans="1:8">
       <c r="A125" s="12" t="str">
-        <f>IF(G125&lt;&gt;"",UPPER(LEFT(G125,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G125,G125),"0000"),"")</f>
+        <f>IF(G125&lt;&gt;"",UPPER(LEFT(G125,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G125,G125),"0000"),"")</f>
         <v/>
       </c>
       <c r="B125" s="5"/>
@@ -3006,7 +3021,7 @@
     </row>
     <row r="126" customHeight="1" spans="1:8">
       <c r="A126" s="12" t="str">
-        <f>IF(G126&lt;&gt;"",UPPER(LEFT(G126,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G126,G126),"0000"),"")</f>
+        <f>IF(G126&lt;&gt;"",UPPER(LEFT(G126,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G126,G126),"0000"),"")</f>
         <v/>
       </c>
       <c r="B126" s="5"/>
@@ -3019,7 +3034,7 @@
     </row>
     <row r="127" customHeight="1" spans="1:8">
       <c r="A127" s="12" t="str">
-        <f>IF(G127&lt;&gt;"",UPPER(LEFT(G127,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G127,G127),"0000"),"")</f>
+        <f>IF(G127&lt;&gt;"",UPPER(LEFT(G127,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G127,G127),"0000"),"")</f>
         <v/>
       </c>
       <c r="B127" s="5"/>
@@ -3032,7 +3047,7 @@
     </row>
     <row r="128" customHeight="1" spans="1:8">
       <c r="A128" s="12" t="str">
-        <f>IF(G128&lt;&gt;"",UPPER(LEFT(G128,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G128,G128),"0000"),"")</f>
+        <f>IF(G128&lt;&gt;"",UPPER(LEFT(G128,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G128,G128),"0000"),"")</f>
         <v/>
       </c>
       <c r="B128" s="5"/>
@@ -3045,7 +3060,7 @@
     </row>
     <row r="129" customHeight="1" spans="1:8">
       <c r="A129" s="12" t="str">
-        <f>IF(G129&lt;&gt;"",UPPER(LEFT(G129,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G129,G129),"0000"),"")</f>
+        <f>IF(G129&lt;&gt;"",UPPER(LEFT(G129,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G129,G129),"0000"),"")</f>
         <v/>
       </c>
       <c r="B129" s="5"/>
@@ -3058,7 +3073,7 @@
     </row>
     <row r="130" customHeight="1" spans="1:8">
       <c r="A130" s="12" t="str">
-        <f>IF(G130&lt;&gt;"",UPPER(LEFT(G130,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G130,G130),"0000"),"")</f>
+        <f>IF(G130&lt;&gt;"",UPPER(LEFT(G130,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G130,G130),"0000"),"")</f>
         <v/>
       </c>
       <c r="B130" s="5"/>
@@ -3071,7 +3086,7 @@
     </row>
     <row r="131" customHeight="1" spans="1:8">
       <c r="A131" s="12" t="str">
-        <f>IF(G131&lt;&gt;"",UPPER(LEFT(G131,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G131,G131),"0000"),"")</f>
+        <f>IF(G131&lt;&gt;"",UPPER(LEFT(G131,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G131,G131),"0000"),"")</f>
         <v/>
       </c>
       <c r="B131" s="5"/>
@@ -3084,7 +3099,7 @@
     </row>
     <row r="132" customHeight="1" spans="1:8">
       <c r="A132" s="12" t="str">
-        <f>IF(G132&lt;&gt;"",UPPER(LEFT(G132,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G132,G132),"0000"),"")</f>
+        <f>IF(G132&lt;&gt;"",UPPER(LEFT(G132,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G132,G132),"0000"),"")</f>
         <v/>
       </c>
       <c r="B132" s="5"/>
@@ -3097,7 +3112,7 @@
     </row>
     <row r="133" customHeight="1" spans="1:8">
       <c r="A133" s="12" t="str">
-        <f>IF(G133&lt;&gt;"",UPPER(LEFT(G133,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G133,G133),"0000"),"")</f>
+        <f>IF(G133&lt;&gt;"",UPPER(LEFT(G133,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G133,G133),"0000"),"")</f>
         <v/>
       </c>
       <c r="B133" s="5"/>
@@ -3110,7 +3125,7 @@
     </row>
     <row r="134" customHeight="1" spans="1:8">
       <c r="A134" s="12" t="str">
-        <f>IF(G134&lt;&gt;"",UPPER(LEFT(G134,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G134,G134),"0000"),"")</f>
+        <f>IF(G134&lt;&gt;"",UPPER(LEFT(G134,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G134,G134),"0000"),"")</f>
         <v/>
       </c>
       <c r="B134" s="5"/>
@@ -3123,7 +3138,7 @@
     </row>
     <row r="135" customHeight="1" spans="1:8">
       <c r="A135" s="12" t="str">
-        <f>IF(G135&lt;&gt;"",UPPER(LEFT(G135,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G135,G135),"0000"),"")</f>
+        <f>IF(G135&lt;&gt;"",UPPER(LEFT(G135,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G135,G135),"0000"),"")</f>
         <v/>
       </c>
       <c r="B135" s="5"/>
@@ -3136,7 +3151,7 @@
     </row>
     <row r="136" customHeight="1" spans="1:8">
       <c r="A136" s="12" t="str">
-        <f>IF(G136&lt;&gt;"",UPPER(LEFT(G136,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G136,G136),"0000"),"")</f>
+        <f>IF(G136&lt;&gt;"",UPPER(LEFT(G136,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G136,G136),"0000"),"")</f>
         <v/>
       </c>
       <c r="B136" s="5"/>
@@ -3149,7 +3164,7 @@
     </row>
     <row r="137" customHeight="1" spans="1:8">
       <c r="A137" s="12" t="str">
-        <f>IF(G137&lt;&gt;"",UPPER(LEFT(G137,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G137,G137),"0000"),"")</f>
+        <f>IF(G137&lt;&gt;"",UPPER(LEFT(G137,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G137,G137),"0000"),"")</f>
         <v/>
       </c>
       <c r="B137" s="5"/>
@@ -3162,7 +3177,7 @@
     </row>
     <row r="138" customHeight="1" spans="1:8">
       <c r="A138" s="12" t="str">
-        <f>IF(G138&lt;&gt;"",UPPER(LEFT(G138,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G138,G138),"0000"),"")</f>
+        <f>IF(G138&lt;&gt;"",UPPER(LEFT(G138,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G138,G138),"0000"),"")</f>
         <v/>
       </c>
       <c r="B138" s="5"/>
@@ -3175,7 +3190,7 @@
     </row>
     <row r="139" customHeight="1" spans="1:8">
       <c r="A139" s="12" t="str">
-        <f>IF(G139&lt;&gt;"",UPPER(LEFT(G139,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G139,G139),"0000"),"")</f>
+        <f>IF(G139&lt;&gt;"",UPPER(LEFT(G139,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G139,G139),"0000"),"")</f>
         <v/>
       </c>
       <c r="B139" s="5"/>
@@ -3188,7 +3203,7 @@
     </row>
     <row r="140" customHeight="1" spans="1:8">
       <c r="A140" s="12" t="str">
-        <f>IF(G140&lt;&gt;"",UPPER(LEFT(G140,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G140,G140),"0000"),"")</f>
+        <f>IF(G140&lt;&gt;"",UPPER(LEFT(G140,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G140,G140),"0000"),"")</f>
         <v/>
       </c>
       <c r="B140" s="5"/>
@@ -3201,7 +3216,7 @@
     </row>
     <row r="141" customHeight="1" spans="1:8">
       <c r="A141" s="12" t="str">
-        <f>IF(G141&lt;&gt;"",UPPER(LEFT(G141,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G141,G141),"0000"),"")</f>
+        <f>IF(G141&lt;&gt;"",UPPER(LEFT(G141,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G141,G141),"0000"),"")</f>
         <v/>
       </c>
       <c r="B141" s="5"/>
@@ -3214,7 +3229,7 @@
     </row>
     <row r="142" customHeight="1" spans="1:8">
       <c r="A142" s="12" t="str">
-        <f>IF(G142&lt;&gt;"",UPPER(LEFT(G142,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G142,G142),"0000"),"")</f>
+        <f>IF(G142&lt;&gt;"",UPPER(LEFT(G142,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G142,G142),"0000"),"")</f>
         <v/>
       </c>
       <c r="B142" s="5"/>
@@ -3227,7 +3242,7 @@
     </row>
     <row r="143" customHeight="1" spans="1:8">
       <c r="A143" s="12" t="str">
-        <f>IF(G143&lt;&gt;"",UPPER(LEFT(G143,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G143,G143),"0000"),"")</f>
+        <f>IF(G143&lt;&gt;"",UPPER(LEFT(G143,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G143,G143),"0000"),"")</f>
         <v/>
       </c>
       <c r="B143" s="5"/>
@@ -3240,7 +3255,7 @@
     </row>
     <row r="144" customHeight="1" spans="1:8">
       <c r="A144" s="12" t="str">
-        <f>IF(G144&lt;&gt;"",UPPER(LEFT(G144,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G144,G144),"0000"),"")</f>
+        <f>IF(G144&lt;&gt;"",UPPER(LEFT(G144,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G144,G144),"0000"),"")</f>
         <v/>
       </c>
       <c r="B144" s="5"/>
@@ -3253,7 +3268,7 @@
     </row>
     <row r="145" customHeight="1" spans="1:8">
       <c r="A145" s="12" t="str">
-        <f>IF(G145&lt;&gt;"",UPPER(LEFT(G145,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G145,G145),"0000"),"")</f>
+        <f>IF(G145&lt;&gt;"",UPPER(LEFT(G145,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G145,G145),"0000"),"")</f>
         <v/>
       </c>
       <c r="B145" s="5"/>
@@ -3266,7 +3281,7 @@
     </row>
     <row r="146" customHeight="1" spans="1:8">
       <c r="A146" s="12" t="str">
-        <f>IF(G146&lt;&gt;"",UPPER(LEFT(G146,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G146,G146),"0000"),"")</f>
+        <f>IF(G146&lt;&gt;"",UPPER(LEFT(G146,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G146,G146),"0000"),"")</f>
         <v/>
       </c>
       <c r="B146" s="5"/>
@@ -3279,7 +3294,7 @@
     </row>
     <row r="147" customHeight="1" spans="1:8">
       <c r="A147" s="12" t="str">
-        <f>IF(G147&lt;&gt;"",UPPER(LEFT(G147,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G147,G147),"0000"),"")</f>
+        <f>IF(G147&lt;&gt;"",UPPER(LEFT(G147,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G147,G147),"0000"),"")</f>
         <v/>
       </c>
       <c r="B147" s="5"/>
@@ -3292,7 +3307,7 @@
     </row>
     <row r="148" customHeight="1" spans="1:8">
       <c r="A148" s="12" t="str">
-        <f>IF(G148&lt;&gt;"",UPPER(LEFT(G148,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G148,G148),"0000"),"")</f>
+        <f>IF(G148&lt;&gt;"",UPPER(LEFT(G148,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G148,G148),"0000"),"")</f>
         <v/>
       </c>
       <c r="B148" s="5"/>
@@ -3305,7 +3320,7 @@
     </row>
     <row r="149" customHeight="1" spans="1:8">
       <c r="A149" s="12" t="str">
-        <f>IF(G149&lt;&gt;"",UPPER(LEFT(G149,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G149,G149),"0000"),"")</f>
+        <f>IF(G149&lt;&gt;"",UPPER(LEFT(G149,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G149,G149),"0000"),"")</f>
         <v/>
       </c>
       <c r="B149" s="5"/>
@@ -3318,7 +3333,7 @@
     </row>
     <row r="150" customHeight="1" spans="1:8">
       <c r="A150" s="12" t="str">
-        <f>IF(G150&lt;&gt;"",UPPER(LEFT(G150,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G150,G150),"0000"),"")</f>
+        <f>IF(G150&lt;&gt;"",UPPER(LEFT(G150,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G150,G150),"0000"),"")</f>
         <v/>
       </c>
       <c r="B150" s="5"/>
@@ -3331,7 +3346,7 @@
     </row>
     <row r="151" customHeight="1" spans="1:8">
       <c r="A151" s="12" t="str">
-        <f>IF(G151&lt;&gt;"",UPPER(LEFT(G151,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G151,G151),"0000"),"")</f>
+        <f>IF(G151&lt;&gt;"",UPPER(LEFT(G151,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G151,G151),"0000"),"")</f>
         <v/>
       </c>
       <c r="B151" s="5"/>
@@ -3344,7 +3359,7 @@
     </row>
     <row r="152" customHeight="1" spans="1:8">
       <c r="A152" s="12" t="str">
-        <f>IF(G152&lt;&gt;"",UPPER(LEFT(G152,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G152,G152),"0000"),"")</f>
+        <f>IF(G152&lt;&gt;"",UPPER(LEFT(G152,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G152,G152),"0000"),"")</f>
         <v/>
       </c>
       <c r="B152" s="5"/>
@@ -3357,7 +3372,7 @@
     </row>
     <row r="153" customHeight="1" spans="1:8">
       <c r="A153" s="12" t="str">
-        <f>IF(G153&lt;&gt;"",UPPER(LEFT(G153,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G153,G153),"0000"),"")</f>
+        <f>IF(G153&lt;&gt;"",UPPER(LEFT(G153,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G153,G153),"0000"),"")</f>
         <v/>
       </c>
       <c r="B153" s="5"/>
@@ -3370,7 +3385,7 @@
     </row>
     <row r="154" customHeight="1" spans="1:8">
       <c r="A154" s="12" t="str">
-        <f>IF(G154&lt;&gt;"",UPPER(LEFT(G154,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G154,G154),"0000"),"")</f>
+        <f>IF(G154&lt;&gt;"",UPPER(LEFT(G154,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G154,G154),"0000"),"")</f>
         <v/>
       </c>
       <c r="B154" s="5"/>
@@ -3383,7 +3398,7 @@
     </row>
     <row r="155" customHeight="1" spans="1:8">
       <c r="A155" s="12" t="str">
-        <f>IF(G155&lt;&gt;"",UPPER(LEFT(G155,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G155,G155),"0000"),"")</f>
+        <f>IF(G155&lt;&gt;"",UPPER(LEFT(G155,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G155,G155),"0000"),"")</f>
         <v/>
       </c>
       <c r="B155" s="5"/>
@@ -3396,7 +3411,7 @@
     </row>
     <row r="156" customHeight="1" spans="1:8">
       <c r="A156" s="12" t="str">
-        <f>IF(G156&lt;&gt;"",UPPER(LEFT(G156,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G156,G156),"0000"),"")</f>
+        <f>IF(G156&lt;&gt;"",UPPER(LEFT(G156,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G156,G156),"0000"),"")</f>
         <v/>
       </c>
       <c r="B156" s="5"/>
@@ -3409,7 +3424,7 @@
     </row>
     <row r="157" customHeight="1" spans="1:8">
       <c r="A157" s="12" t="str">
-        <f>IF(G157&lt;&gt;"",UPPER(LEFT(G157,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G157,G157),"0000"),"")</f>
+        <f>IF(G157&lt;&gt;"",UPPER(LEFT(G157,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G157,G157),"0000"),"")</f>
         <v/>
       </c>
       <c r="B157" s="5"/>
@@ -3422,7 +3437,7 @@
     </row>
     <row r="158" customHeight="1" spans="1:8">
       <c r="A158" s="12" t="str">
-        <f>IF(G158&lt;&gt;"",UPPER(LEFT(G158,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G158,G158),"0000"),"")</f>
+        <f>IF(G158&lt;&gt;"",UPPER(LEFT(G158,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G158,G158),"0000"),"")</f>
         <v/>
       </c>
       <c r="B158" s="5"/>
@@ -3435,7 +3450,7 @@
     </row>
     <row r="159" customHeight="1" spans="1:8">
       <c r="A159" s="12" t="str">
-        <f>IF(G159&lt;&gt;"",UPPER(LEFT(G159,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G159,G159),"0000"),"")</f>
+        <f>IF(G159&lt;&gt;"",UPPER(LEFT(G159,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G159,G159),"0000"),"")</f>
         <v/>
       </c>
       <c r="B159" s="5"/>
@@ -3448,7 +3463,7 @@
     </row>
     <row r="160" customHeight="1" spans="1:8">
       <c r="A160" s="12" t="str">
-        <f>IF(G160&lt;&gt;"",UPPER(LEFT(G160,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G160,G160),"0000"),"")</f>
+        <f>IF(G160&lt;&gt;"",UPPER(LEFT(G160,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G160,G160),"0000"),"")</f>
         <v/>
       </c>
       <c r="B160" s="5"/>
@@ -3461,7 +3476,7 @@
     </row>
     <row r="161" customHeight="1" spans="1:8">
       <c r="A161" s="12" t="str">
-        <f>IF(G161&lt;&gt;"",UPPER(LEFT(G161,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G161,G161),"0000"),"")</f>
+        <f>IF(G161&lt;&gt;"",UPPER(LEFT(G161,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G161,G161),"0000"),"")</f>
         <v/>
       </c>
       <c r="B161" s="5"/>
@@ -3474,7 +3489,7 @@
     </row>
     <row r="162" customHeight="1" spans="1:8">
       <c r="A162" s="12" t="str">
-        <f>IF(G162&lt;&gt;"",UPPER(LEFT(G162,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G162,G162),"0000"),"")</f>
+        <f>IF(G162&lt;&gt;"",UPPER(LEFT(G162,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G162,G162),"0000"),"")</f>
         <v/>
       </c>
       <c r="B162" s="5"/>
@@ -3487,7 +3502,7 @@
     </row>
     <row r="163" customHeight="1" spans="1:8">
       <c r="A163" s="12" t="str">
-        <f>IF(G163&lt;&gt;"",UPPER(LEFT(G163,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G163,G163),"0000"),"")</f>
+        <f>IF(G163&lt;&gt;"",UPPER(LEFT(G163,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G163,G163),"0000"),"")</f>
         <v/>
       </c>
       <c r="B163" s="5"/>
@@ -3500,7 +3515,7 @@
     </row>
     <row r="164" customHeight="1" spans="1:8">
       <c r="A164" s="12" t="str">
-        <f>IF(G164&lt;&gt;"",UPPER(LEFT(G164,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G164,G164),"0000"),"")</f>
+        <f>IF(G164&lt;&gt;"",UPPER(LEFT(G164,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G164,G164),"0000"),"")</f>
         <v/>
       </c>
       <c r="B164" s="5"/>
@@ -3513,7 +3528,7 @@
     </row>
     <row r="165" customHeight="1" spans="1:8">
       <c r="A165" s="12" t="str">
-        <f>IF(G165&lt;&gt;"",UPPER(LEFT(G165,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G165,G165),"0000"),"")</f>
+        <f>IF(G165&lt;&gt;"",UPPER(LEFT(G165,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G165,G165),"0000"),"")</f>
         <v/>
       </c>
       <c r="B165" s="5"/>
@@ -3526,7 +3541,7 @@
     </row>
     <row r="166" customHeight="1" spans="1:8">
       <c r="A166" s="12" t="str">
-        <f>IF(G166&lt;&gt;"",UPPER(LEFT(G166,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G166,G166),"0000"),"")</f>
+        <f>IF(G166&lt;&gt;"",UPPER(LEFT(G166,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G166,G166),"0000"),"")</f>
         <v/>
       </c>
       <c r="B166" s="5"/>
@@ -3539,7 +3554,7 @@
     </row>
     <row r="167" customHeight="1" spans="1:8">
       <c r="A167" s="12" t="str">
-        <f>IF(G167&lt;&gt;"",UPPER(LEFT(G167,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G167,G167),"0000"),"")</f>
+        <f>IF(G167&lt;&gt;"",UPPER(LEFT(G167,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G167,G167),"0000"),"")</f>
         <v/>
       </c>
       <c r="B167" s="5"/>
@@ -3552,7 +3567,7 @@
     </row>
     <row r="168" customHeight="1" spans="1:8">
       <c r="A168" s="12" t="str">
-        <f>IF(G168&lt;&gt;"",UPPER(LEFT(G168,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G168,G168),"0000"),"")</f>
+        <f>IF(G168&lt;&gt;"",UPPER(LEFT(G168,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G168,G168),"0000"),"")</f>
         <v/>
       </c>
       <c r="B168" s="5"/>
@@ -3565,7 +3580,7 @@
     </row>
     <row r="169" customHeight="1" spans="1:8">
       <c r="A169" s="12" t="str">
-        <f>IF(G169&lt;&gt;"",UPPER(LEFT(G169,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G169,G169),"0000"),"")</f>
+        <f>IF(G169&lt;&gt;"",UPPER(LEFT(G169,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G169,G169),"0000"),"")</f>
         <v/>
       </c>
       <c r="B169" s="5"/>
@@ -3578,7 +3593,7 @@
     </row>
     <row r="170" customHeight="1" spans="1:8">
       <c r="A170" s="12" t="str">
-        <f>IF(G170&lt;&gt;"",UPPER(LEFT(G170,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G170,G170),"0000"),"")</f>
+        <f>IF(G170&lt;&gt;"",UPPER(LEFT(G170,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G170,G170),"0000"),"")</f>
         <v/>
       </c>
       <c r="B170" s="5"/>
@@ -3591,7 +3606,7 @@
     </row>
     <row r="171" customHeight="1" spans="1:8">
       <c r="A171" s="12" t="str">
-        <f>IF(G171&lt;&gt;"",UPPER(LEFT(G171,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G171,G171),"0000"),"")</f>
+        <f>IF(G171&lt;&gt;"",UPPER(LEFT(G171,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G171,G171),"0000"),"")</f>
         <v/>
       </c>
       <c r="B171" s="5"/>
@@ -3604,7 +3619,7 @@
     </row>
     <row r="172" customHeight="1" spans="1:8">
       <c r="A172" s="12" t="str">
-        <f>IF(G172&lt;&gt;"",UPPER(LEFT(G172,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G172,G172),"0000"),"")</f>
+        <f>IF(G172&lt;&gt;"",UPPER(LEFT(G172,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G172,G172),"0000"),"")</f>
         <v/>
       </c>
       <c r="B172" s="5"/>
@@ -3617,7 +3632,7 @@
     </row>
     <row r="173" customHeight="1" spans="1:8">
       <c r="A173" s="12" t="str">
-        <f>IF(G173&lt;&gt;"",UPPER(LEFT(G173,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G173,G173),"0000"),"")</f>
+        <f>IF(G173&lt;&gt;"",UPPER(LEFT(G173,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G173,G173),"0000"),"")</f>
         <v/>
       </c>
       <c r="B173" s="5"/>
@@ -3630,7 +3645,7 @@
     </row>
     <row r="174" customHeight="1" spans="1:8">
       <c r="A174" s="12" t="str">
-        <f>IF(G174&lt;&gt;"",UPPER(LEFT(G174,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G174,G174),"0000"),"")</f>
+        <f>IF(G174&lt;&gt;"",UPPER(LEFT(G174,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G174,G174),"0000"),"")</f>
         <v/>
       </c>
       <c r="B174" s="5"/>
@@ -3643,7 +3658,7 @@
     </row>
     <row r="175" customHeight="1" spans="1:8">
       <c r="A175" s="12" t="str">
-        <f>IF(G175&lt;&gt;"",UPPER(LEFT(G175,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G175,G175),"0000"),"")</f>
+        <f>IF(G175&lt;&gt;"",UPPER(LEFT(G175,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G175,G175),"0000"),"")</f>
         <v/>
       </c>
       <c r="B175" s="5"/>
@@ -3656,7 +3671,7 @@
     </row>
     <row r="176" customHeight="1" spans="1:8">
       <c r="A176" s="12" t="str">
-        <f>IF(G176&lt;&gt;"",UPPER(LEFT(G176,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G176,G176),"0000"),"")</f>
+        <f>IF(G176&lt;&gt;"",UPPER(LEFT(G176,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G176,G176),"0000"),"")</f>
         <v/>
       </c>
       <c r="B176" s="5"/>
@@ -3669,7 +3684,7 @@
     </row>
     <row r="177" customHeight="1" spans="1:8">
       <c r="A177" s="12" t="str">
-        <f>IF(G177&lt;&gt;"",UPPER(LEFT(G177,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G177,G177),"0000"),"")</f>
+        <f>IF(G177&lt;&gt;"",UPPER(LEFT(G177,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G177,G177),"0000"),"")</f>
         <v/>
       </c>
       <c r="B177" s="5"/>
@@ -3682,7 +3697,7 @@
     </row>
     <row r="178" customHeight="1" spans="1:8">
       <c r="A178" s="12" t="str">
-        <f>IF(G178&lt;&gt;"",UPPER(LEFT(G178,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G178,G178),"0000"),"")</f>
+        <f>IF(G178&lt;&gt;"",UPPER(LEFT(G178,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G178,G178),"0000"),"")</f>
         <v/>
       </c>
       <c r="B178" s="5"/>
@@ -3695,7 +3710,7 @@
     </row>
     <row r="179" customHeight="1" spans="1:8">
       <c r="A179" s="12" t="str">
-        <f>IF(G179&lt;&gt;"",UPPER(LEFT(G179,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G179,G179),"0000"),"")</f>
+        <f>IF(G179&lt;&gt;"",UPPER(LEFT(G179,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G179,G179),"0000"),"")</f>
         <v/>
       </c>
       <c r="B179" s="5"/>
@@ -3708,7 +3723,7 @@
     </row>
     <row r="180" customHeight="1" spans="1:8">
       <c r="A180" s="12" t="str">
-        <f>IF(G180&lt;&gt;"",UPPER(LEFT(G180,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G180,G180),"0000"),"")</f>
+        <f>IF(G180&lt;&gt;"",UPPER(LEFT(G180,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G180,G180),"0000"),"")</f>
         <v/>
       </c>
       <c r="B180" s="5"/>
@@ -3721,7 +3736,7 @@
     </row>
     <row r="181" customHeight="1" spans="1:8">
       <c r="A181" s="12" t="str">
-        <f>IF(G181&lt;&gt;"",UPPER(LEFT(G181,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G181,G181),"0000"),"")</f>
+        <f>IF(G181&lt;&gt;"",UPPER(LEFT(G181,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G181,G181),"0000"),"")</f>
         <v/>
       </c>
       <c r="B181" s="5"/>
@@ -3734,7 +3749,7 @@
     </row>
     <row r="182" customHeight="1" spans="1:8">
       <c r="A182" s="12" t="str">
-        <f>IF(G182&lt;&gt;"",UPPER(LEFT(G182,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G182,G182),"0000"),"")</f>
+        <f>IF(G182&lt;&gt;"",UPPER(LEFT(G182,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G182,G182),"0000"),"")</f>
         <v/>
       </c>
       <c r="B182" s="5"/>
@@ -3747,7 +3762,7 @@
     </row>
     <row r="183" customHeight="1" spans="1:8">
       <c r="A183" s="12" t="str">
-        <f>IF(G183&lt;&gt;"",UPPER(LEFT(G183,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G183,G183),"0000"),"")</f>
+        <f>IF(G183&lt;&gt;"",UPPER(LEFT(G183,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G183,G183),"0000"),"")</f>
         <v/>
       </c>
       <c r="B183" s="5"/>
@@ -3760,7 +3775,7 @@
     </row>
     <row r="184" customHeight="1" spans="1:8">
       <c r="A184" s="12" t="str">
-        <f>IF(G184&lt;&gt;"",UPPER(LEFT(G184,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G184,G184),"0000"),"")</f>
+        <f>IF(G184&lt;&gt;"",UPPER(LEFT(G184,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G184,G184),"0000"),"")</f>
         <v/>
       </c>
       <c r="B184" s="5"/>
@@ -3773,7 +3788,7 @@
     </row>
     <row r="185" customHeight="1" spans="1:8">
       <c r="A185" s="12" t="str">
-        <f>IF(G185&lt;&gt;"",UPPER(LEFT(G185,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G185,G185),"0000"),"")</f>
+        <f>IF(G185&lt;&gt;"",UPPER(LEFT(G185,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G185,G185),"0000"),"")</f>
         <v/>
       </c>
       <c r="B185" s="5"/>
@@ -3786,7 +3801,7 @@
     </row>
     <row r="186" customHeight="1" spans="1:8">
       <c r="A186" s="12" t="str">
-        <f>IF(G186&lt;&gt;"",UPPER(LEFT(G186,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G186,G186),"0000"),"")</f>
+        <f>IF(G186&lt;&gt;"",UPPER(LEFT(G186,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G186,G186),"0000"),"")</f>
         <v/>
       </c>
       <c r="B186" s="5"/>
@@ -3799,7 +3814,7 @@
     </row>
     <row r="187" customHeight="1" spans="1:8">
       <c r="A187" s="12" t="str">
-        <f>IF(G187&lt;&gt;"",UPPER(LEFT(G187,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G187,G187),"0000"),"")</f>
+        <f>IF(G187&lt;&gt;"",UPPER(LEFT(G187,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G187,G187),"0000"),"")</f>
         <v/>
       </c>
       <c r="B187" s="5"/>
@@ -3812,7 +3827,7 @@
     </row>
     <row r="188" customHeight="1" spans="1:8">
       <c r="A188" s="12" t="str">
-        <f>IF(G188&lt;&gt;"",UPPER(LEFT(G188,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G188,G188),"0000"),"")</f>
+        <f>IF(G188&lt;&gt;"",UPPER(LEFT(G188,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G188,G188),"0000"),"")</f>
         <v/>
       </c>
       <c r="B188" s="5"/>
@@ -3825,7 +3840,7 @@
     </row>
     <row r="189" customHeight="1" spans="1:8">
       <c r="A189" s="12" t="str">
-        <f>IF(G189&lt;&gt;"",UPPER(LEFT(G189,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G189,G189),"0000"),"")</f>
+        <f>IF(G189&lt;&gt;"",UPPER(LEFT(G189,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G189,G189),"0000"),"")</f>
         <v/>
       </c>
       <c r="B189" s="5"/>
@@ -3838,7 +3853,7 @@
     </row>
     <row r="190" customHeight="1" spans="1:8">
       <c r="A190" s="12" t="str">
-        <f>IF(G190&lt;&gt;"",UPPER(LEFT(G190,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G190,G190),"0000"),"")</f>
+        <f>IF(G190&lt;&gt;"",UPPER(LEFT(G190,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G190,G190),"0000"),"")</f>
         <v/>
       </c>
       <c r="B190" s="5"/>
@@ -3851,7 +3866,7 @@
     </row>
     <row r="191" customHeight="1" spans="1:8">
       <c r="A191" s="12" t="str">
-        <f>IF(G191&lt;&gt;"",UPPER(LEFT(G191,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G191,G191),"0000"),"")</f>
+        <f>IF(G191&lt;&gt;"",UPPER(LEFT(G191,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G191,G191),"0000"),"")</f>
         <v/>
       </c>
       <c r="B191" s="5"/>
@@ -3864,7 +3879,7 @@
     </row>
     <row r="192" customHeight="1" spans="1:8">
       <c r="A192" s="12" t="str">
-        <f>IF(G192&lt;&gt;"",UPPER(LEFT(G192,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G192,G192),"0000"),"")</f>
+        <f>IF(G192&lt;&gt;"",UPPER(LEFT(G192,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G192,G192),"0000"),"")</f>
         <v/>
       </c>
       <c r="B192" s="5"/>
@@ -3877,7 +3892,7 @@
     </row>
     <row r="193" customHeight="1" spans="1:8">
       <c r="A193" s="12" t="str">
-        <f>IF(G193&lt;&gt;"",UPPER(LEFT(G193,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G193,G193),"0000"),"")</f>
+        <f>IF(G193&lt;&gt;"",UPPER(LEFT(G193,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G193,G193),"0000"),"")</f>
         <v/>
       </c>
       <c r="B193" s="5"/>
@@ -3890,7 +3905,7 @@
     </row>
     <row r="194" customHeight="1" spans="1:8">
       <c r="A194" s="12" t="str">
-        <f>IF(G194&lt;&gt;"",UPPER(LEFT(G194,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G194,G194),"0000"),"")</f>
+        <f>IF(G194&lt;&gt;"",UPPER(LEFT(G194,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G194,G194),"0000"),"")</f>
         <v/>
       </c>
       <c r="B194" s="5"/>
@@ -3903,7 +3918,7 @@
     </row>
     <row r="195" customHeight="1" spans="1:8">
       <c r="A195" s="12" t="str">
-        <f>IF(G195&lt;&gt;"",UPPER(LEFT(G195,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G195,G195),"0000"),"")</f>
+        <f>IF(G195&lt;&gt;"",UPPER(LEFT(G195,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G195,G195),"0000"),"")</f>
         <v/>
       </c>
       <c r="B195" s="5"/>
@@ -3916,7 +3931,7 @@
     </row>
     <row r="196" customHeight="1" spans="1:8">
       <c r="A196" s="12" t="str">
-        <f>IF(G196&lt;&gt;"",UPPER(LEFT(G196,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G196,G196),"0000"),"")</f>
+        <f>IF(G196&lt;&gt;"",UPPER(LEFT(G196,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G196,G196),"0000"),"")</f>
         <v/>
       </c>
       <c r="B196" s="5"/>
@@ -3929,7 +3944,7 @@
     </row>
     <row r="197" customHeight="1" spans="1:8">
       <c r="A197" s="12" t="str">
-        <f>IF(G197&lt;&gt;"",UPPER(LEFT(G197,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G197,G197),"0000"),"")</f>
+        <f>IF(G197&lt;&gt;"",UPPER(LEFT(G197,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G197,G197),"0000"),"")</f>
         <v/>
       </c>
       <c r="B197" s="5"/>
@@ -3942,7 +3957,7 @@
     </row>
     <row r="198" customHeight="1" spans="1:8">
       <c r="A198" s="12" t="str">
-        <f>IF(G198&lt;&gt;"",UPPER(LEFT(G198,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G198,G198),"0000"),"")</f>
+        <f>IF(G198&lt;&gt;"",UPPER(LEFT(G198,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G198,G198),"0000"),"")</f>
         <v/>
       </c>
       <c r="B198" s="5"/>
@@ -3955,7 +3970,7 @@
     </row>
     <row r="199" customHeight="1" spans="1:8">
       <c r="A199" s="12" t="str">
-        <f>IF(G199&lt;&gt;"",UPPER(LEFT(G199,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G199,G199),"0000"),"")</f>
+        <f>IF(G199&lt;&gt;"",UPPER(LEFT(G199,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G199,G199),"0000"),"")</f>
         <v/>
       </c>
       <c r="B199" s="5"/>
@@ -3968,7 +3983,7 @@
     </row>
     <row r="200" customHeight="1" spans="1:8">
       <c r="A200" s="12" t="str">
-        <f>IF(G200&lt;&gt;"",UPPER(LEFT(G200,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G200,G200),"0000"),"")</f>
+        <f>IF(G200&lt;&gt;"",UPPER(LEFT(G200,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G200,G200),"0000"),"")</f>
         <v/>
       </c>
       <c r="B200" s="5"/>
@@ -3981,7 +3996,7 @@
     </row>
     <row r="201" customHeight="1" spans="1:8">
       <c r="A201" s="12" t="str">
-        <f>IF(G201&lt;&gt;"",UPPER(LEFT(G201,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G201,G201),"0000"),"")</f>
+        <f>IF(G201&lt;&gt;"",UPPER(LEFT(G201,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G201,G201),"0000"),"")</f>
         <v/>
       </c>
       <c r="B201" s="5"/>
@@ -3994,7 +4009,7 @@
     </row>
     <row r="202" customHeight="1" spans="1:8">
       <c r="A202" s="12" t="str">
-        <f>IF(G202&lt;&gt;"",UPPER(LEFT(G202,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G202,G202),"0000"),"")</f>
+        <f>IF(G202&lt;&gt;"",UPPER(LEFT(G202,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G202,G202),"0000"),"")</f>
         <v/>
       </c>
       <c r="B202" s="5"/>
@@ -4007,7 +4022,7 @@
     </row>
     <row r="203" customHeight="1" spans="1:8">
       <c r="A203" s="12" t="str">
-        <f>IF(G203&lt;&gt;"",UPPER(LEFT(G203,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G203,G203),"0000"),"")</f>
+        <f>IF(G203&lt;&gt;"",UPPER(LEFT(G203,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G203,G203),"0000"),"")</f>
         <v/>
       </c>
       <c r="B203" s="5"/>
@@ -4020,7 +4035,7 @@
     </row>
     <row r="204" customHeight="1" spans="1:8">
       <c r="A204" s="12" t="str">
-        <f>IF(G204&lt;&gt;"",UPPER(LEFT(G204,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G204,G204),"0000"),"")</f>
+        <f>IF(G204&lt;&gt;"",UPPER(LEFT(G204,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G204,G204),"0000"),"")</f>
         <v/>
       </c>
       <c r="B204" s="5"/>
@@ -4033,7 +4048,7 @@
     </row>
     <row r="205" customHeight="1" spans="1:8">
       <c r="A205" s="12" t="str">
-        <f>IF(G205&lt;&gt;"",UPPER(LEFT(G205,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G205,G205),"0000"),"")</f>
+        <f>IF(G205&lt;&gt;"",UPPER(LEFT(G205,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G205,G205),"0000"),"")</f>
         <v/>
       </c>
       <c r="B205" s="5"/>
@@ -4046,7 +4061,7 @@
     </row>
     <row r="206" customHeight="1" spans="1:8">
       <c r="A206" s="12" t="str">
-        <f>IF(G206&lt;&gt;"",UPPER(LEFT(G206,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G206,G206),"0000"),"")</f>
+        <f>IF(G206&lt;&gt;"",UPPER(LEFT(G206,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G206,G206),"0000"),"")</f>
         <v/>
       </c>
       <c r="B206" s="5"/>
@@ -4059,7 +4074,7 @@
     </row>
     <row r="207" customHeight="1" spans="1:8">
       <c r="A207" s="12" t="str">
-        <f>IF(G207&lt;&gt;"",UPPER(LEFT(G207,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G207,G207),"0000"),"")</f>
+        <f>IF(G207&lt;&gt;"",UPPER(LEFT(G207,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G207,G207),"0000"),"")</f>
         <v/>
       </c>
       <c r="B207" s="5"/>
@@ -4072,7 +4087,7 @@
     </row>
     <row r="208" customHeight="1" spans="1:8">
       <c r="A208" s="12" t="str">
-        <f>IF(G208&lt;&gt;"",UPPER(LEFT(G208,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G208,G208),"0000"),"")</f>
+        <f>IF(G208&lt;&gt;"",UPPER(LEFT(G208,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G208,G208),"0000"),"")</f>
         <v/>
       </c>
       <c r="B208" s="5"/>
@@ -4085,7 +4100,7 @@
     </row>
     <row r="209" customHeight="1" spans="1:8">
       <c r="A209" s="12" t="str">
-        <f>IF(G209&lt;&gt;"",UPPER(LEFT(G209,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G209,G209),"0000"),"")</f>
+        <f>IF(G209&lt;&gt;"",UPPER(LEFT(G209,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G209,G209),"0000"),"")</f>
         <v/>
       </c>
       <c r="B209" s="5"/>
@@ -4098,7 +4113,7 @@
     </row>
     <row r="210" customHeight="1" spans="1:8">
       <c r="A210" s="12" t="str">
-        <f>IF(G210&lt;&gt;"",UPPER(LEFT(G210,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G210,G210),"0000"),"")</f>
+        <f>IF(G210&lt;&gt;"",UPPER(LEFT(G210,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G210,G210),"0000"),"")</f>
         <v/>
       </c>
       <c r="B210" s="5"/>
@@ -4111,7 +4126,7 @@
     </row>
     <row r="211" customHeight="1" spans="1:8">
       <c r="A211" s="12" t="str">
-        <f>IF(G211&lt;&gt;"",UPPER(LEFT(G211,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G211,G211),"0000"),"")</f>
+        <f>IF(G211&lt;&gt;"",UPPER(LEFT(G211,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G211,G211),"0000"),"")</f>
         <v/>
       </c>
       <c r="B211" s="5"/>
@@ -4124,7 +4139,7 @@
     </row>
     <row r="212" customHeight="1" spans="1:8">
       <c r="A212" s="12" t="str">
-        <f>IF(G212&lt;&gt;"",UPPER(LEFT(G212,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G212,G212),"0000"),"")</f>
+        <f>IF(G212&lt;&gt;"",UPPER(LEFT(G212,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G212,G212),"0000"),"")</f>
         <v/>
       </c>
       <c r="B212" s="5"/>
@@ -4137,7 +4152,7 @@
     </row>
     <row r="213" customHeight="1" spans="1:8">
       <c r="A213" s="12" t="str">
-        <f>IF(G213&lt;&gt;"",UPPER(LEFT(G213,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G213,G213),"0000"),"")</f>
+        <f>IF(G213&lt;&gt;"",UPPER(LEFT(G213,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G213,G213),"0000"),"")</f>
         <v/>
       </c>
       <c r="B213" s="5"/>
@@ -4150,7 +4165,7 @@
     </row>
     <row r="214" customHeight="1" spans="1:8">
       <c r="A214" s="12" t="str">
-        <f>IF(G214&lt;&gt;"",UPPER(LEFT(G214,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G214,G214),"0000"),"")</f>
+        <f>IF(G214&lt;&gt;"",UPPER(LEFT(G214,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G214,G214),"0000"),"")</f>
         <v/>
       </c>
       <c r="B214" s="5"/>
@@ -4163,7 +4178,7 @@
     </row>
     <row r="215" customHeight="1" spans="1:8">
       <c r="A215" s="12" t="str">
-        <f>IF(G215&lt;&gt;"",UPPER(LEFT(G215,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G215,G215),"0000"),"")</f>
+        <f>IF(G215&lt;&gt;"",UPPER(LEFT(G215,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G215,G215),"0000"),"")</f>
         <v/>
       </c>
       <c r="B215" s="5"/>
@@ -4176,7 +4191,7 @@
     </row>
     <row r="216" customHeight="1" spans="1:8">
       <c r="A216" s="12" t="str">
-        <f>IF(G216&lt;&gt;"",UPPER(LEFT(G216,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G216,G216),"0000"),"")</f>
+        <f>IF(G216&lt;&gt;"",UPPER(LEFT(G216,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G216,G216),"0000"),"")</f>
         <v/>
       </c>
       <c r="B216" s="5"/>
@@ -4189,7 +4204,7 @@
     </row>
     <row r="217" customHeight="1" spans="1:8">
       <c r="A217" s="12" t="str">
-        <f>IF(G217&lt;&gt;"",UPPER(LEFT(G217,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G217,G217),"0000"),"")</f>
+        <f>IF(G217&lt;&gt;"",UPPER(LEFT(G217,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G217,G217),"0000"),"")</f>
         <v/>
       </c>
       <c r="B217" s="5"/>
@@ -4202,7 +4217,7 @@
     </row>
     <row r="218" customHeight="1" spans="1:8">
       <c r="A218" s="12" t="str">
-        <f>IF(G218&lt;&gt;"",UPPER(LEFT(G218,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G218,G218),"0000"),"")</f>
+        <f>IF(G218&lt;&gt;"",UPPER(LEFT(G218,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G218,G218),"0000"),"")</f>
         <v/>
       </c>
       <c r="B218" s="5"/>
@@ -4215,7 +4230,7 @@
     </row>
     <row r="219" customHeight="1" spans="1:8">
       <c r="A219" s="12" t="str">
-        <f>IF(G219&lt;&gt;"",UPPER(LEFT(G219,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G219,G219),"0000"),"")</f>
+        <f>IF(G219&lt;&gt;"",UPPER(LEFT(G219,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G219,G219),"0000"),"")</f>
         <v/>
       </c>
       <c r="B219" s="5"/>
@@ -4228,7 +4243,7 @@
     </row>
     <row r="220" customHeight="1" spans="1:8">
       <c r="A220" s="12" t="str">
-        <f>IF(G220&lt;&gt;"",UPPER(LEFT(G220,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G220,G220),"0000"),"")</f>
+        <f>IF(G220&lt;&gt;"",UPPER(LEFT(G220,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G220,G220),"0000"),"")</f>
         <v/>
       </c>
       <c r="B220" s="5"/>
@@ -4241,7 +4256,7 @@
     </row>
     <row r="221" customHeight="1" spans="1:8">
       <c r="A221" s="12" t="str">
-        <f>IF(G221&lt;&gt;"",UPPER(LEFT(G221,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G221,G221),"0000"),"")</f>
+        <f>IF(G221&lt;&gt;"",UPPER(LEFT(G221,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G221,G221),"0000"),"")</f>
         <v/>
       </c>
       <c r="B221" s="5"/>
@@ -4254,7 +4269,7 @@
     </row>
     <row r="222" customHeight="1" spans="1:8">
       <c r="A222" s="12" t="str">
-        <f>IF(G222&lt;&gt;"",UPPER(LEFT(G222,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G222,G222),"0000"),"")</f>
+        <f>IF(G222&lt;&gt;"",UPPER(LEFT(G222,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G222,G222),"0000"),"")</f>
         <v/>
       </c>
       <c r="B222" s="5"/>
@@ -4267,7 +4282,7 @@
     </row>
     <row r="223" customHeight="1" spans="1:8">
       <c r="A223" s="12" t="str">
-        <f>IF(G223&lt;&gt;"",UPPER(LEFT(G223,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G223,G223),"0000"),"")</f>
+        <f>IF(G223&lt;&gt;"",UPPER(LEFT(G223,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G223,G223),"0000"),"")</f>
         <v/>
       </c>
       <c r="B223" s="5"/>
@@ -4280,7 +4295,7 @@
     </row>
     <row r="224" customHeight="1" spans="1:8">
       <c r="A224" s="12" t="str">
-        <f>IF(G224&lt;&gt;"",UPPER(LEFT(G224,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G224,G224),"0000"),"")</f>
+        <f>IF(G224&lt;&gt;"",UPPER(LEFT(G224,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G224,G224),"0000"),"")</f>
         <v/>
       </c>
       <c r="B224" s="5"/>
@@ -4293,7 +4308,7 @@
     </row>
     <row r="225" customHeight="1" spans="1:8">
       <c r="A225" s="12" t="str">
-        <f>IF(G225&lt;&gt;"",UPPER(LEFT(G225,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G225,G225),"0000"),"")</f>
+        <f>IF(G225&lt;&gt;"",UPPER(LEFT(G225,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G225,G225),"0000"),"")</f>
         <v/>
       </c>
       <c r="B225" s="5"/>
@@ -4306,7 +4321,7 @@
     </row>
     <row r="226" customHeight="1" spans="1:8">
       <c r="A226" s="12" t="str">
-        <f>IF(G226&lt;&gt;"",UPPER(LEFT(G226,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G226,G226),"0000"),"")</f>
+        <f>IF(G226&lt;&gt;"",UPPER(LEFT(G226,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G226,G226),"0000"),"")</f>
         <v/>
       </c>
       <c r="B226" s="5"/>
@@ -4319,7 +4334,7 @@
     </row>
     <row r="227" customHeight="1" spans="1:8">
       <c r="A227" s="12" t="str">
-        <f>IF(G227&lt;&gt;"",UPPER(LEFT(G227,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G227,G227),"0000"),"")</f>
+        <f>IF(G227&lt;&gt;"",UPPER(LEFT(G227,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G227,G227),"0000"),"")</f>
         <v/>
       </c>
       <c r="B227" s="5"/>
@@ -4332,7 +4347,7 @@
     </row>
     <row r="228" customHeight="1" spans="1:8">
       <c r="A228" s="12" t="str">
-        <f>IF(G228&lt;&gt;"",UPPER(LEFT(G228,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G228,G228),"0000"),"")</f>
+        <f>IF(G228&lt;&gt;"",UPPER(LEFT(G228,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G228,G228),"0000"),"")</f>
         <v/>
       </c>
       <c r="B228" s="5"/>
@@ -4345,7 +4360,7 @@
     </row>
     <row r="229" customHeight="1" spans="1:8">
       <c r="A229" s="12" t="str">
-        <f>IF(G229&lt;&gt;"",UPPER(LEFT(G229,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G229,G229),"0000"),"")</f>
+        <f>IF(G229&lt;&gt;"",UPPER(LEFT(G229,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G229,G229),"0000"),"")</f>
         <v/>
       </c>
       <c r="B229" s="5"/>
@@ -4358,7 +4373,7 @@
     </row>
     <row r="230" customHeight="1" spans="1:8">
       <c r="A230" s="12" t="str">
-        <f>IF(G230&lt;&gt;"",UPPER(LEFT(G230,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G230,G230),"0000"),"")</f>
+        <f>IF(G230&lt;&gt;"",UPPER(LEFT(G230,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G230,G230),"0000"),"")</f>
         <v/>
       </c>
       <c r="B230" s="5"/>
@@ -4371,7 +4386,7 @@
     </row>
     <row r="231" customHeight="1" spans="1:8">
       <c r="A231" s="12" t="str">
-        <f>IF(G231&lt;&gt;"",UPPER(LEFT(G231,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G231,G231),"0000"),"")</f>
+        <f>IF(G231&lt;&gt;"",UPPER(LEFT(G231,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G231,G231),"0000"),"")</f>
         <v/>
       </c>
       <c r="B231" s="5"/>
@@ -4384,7 +4399,7 @@
     </row>
     <row r="232" customHeight="1" spans="1:8">
       <c r="A232" s="12" t="str">
-        <f>IF(G232&lt;&gt;"",UPPER(LEFT(G232,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G232,G232),"0000"),"")</f>
+        <f>IF(G232&lt;&gt;"",UPPER(LEFT(G232,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G232,G232),"0000"),"")</f>
         <v/>
       </c>
       <c r="B232" s="5"/>
@@ -4397,7 +4412,7 @@
     </row>
     <row r="233" customHeight="1" spans="1:8">
       <c r="A233" s="12" t="str">
-        <f>IF(G233&lt;&gt;"",UPPER(LEFT(G233,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G233,G233),"0000"),"")</f>
+        <f>IF(G233&lt;&gt;"",UPPER(LEFT(G233,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G233,G233),"0000"),"")</f>
         <v/>
       </c>
       <c r="B233" s="5"/>
@@ -4410,7 +4425,7 @@
     </row>
     <row r="234" customHeight="1" spans="1:8">
       <c r="A234" s="12" t="str">
-        <f>IF(G234&lt;&gt;"",UPPER(LEFT(G234,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G234,G234),"0000"),"")</f>
+        <f>IF(G234&lt;&gt;"",UPPER(LEFT(G234,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G234,G234),"0000"),"")</f>
         <v/>
       </c>
       <c r="B234" s="5"/>
@@ -4423,7 +4438,7 @@
     </row>
     <row r="235" customHeight="1" spans="1:8">
       <c r="A235" s="12" t="str">
-        <f>IF(G235&lt;&gt;"",UPPER(LEFT(G235,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G235,G235),"0000"),"")</f>
+        <f>IF(G235&lt;&gt;"",UPPER(LEFT(G235,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G235,G235),"0000"),"")</f>
         <v/>
       </c>
       <c r="B235" s="5"/>
@@ -4436,7 +4451,7 @@
     </row>
     <row r="236" customHeight="1" spans="1:8">
       <c r="A236" s="12" t="str">
-        <f>IF(G236&lt;&gt;"",UPPER(LEFT(G236,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G236,G236),"0000"),"")</f>
+        <f>IF(G236&lt;&gt;"",UPPER(LEFT(G236,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G236,G236),"0000"),"")</f>
         <v/>
       </c>
       <c r="B236" s="5"/>
@@ -4449,7 +4464,7 @@
     </row>
     <row r="237" customHeight="1" spans="1:8">
       <c r="A237" s="12" t="str">
-        <f>IF(G237&lt;&gt;"",UPPER(LEFT(G237,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G237,G237),"0000"),"")</f>
+        <f>IF(G237&lt;&gt;"",UPPER(LEFT(G237,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G237,G237),"0000"),"")</f>
         <v/>
       </c>
       <c r="B237" s="5"/>
@@ -4462,7 +4477,7 @@
     </row>
     <row r="238" customHeight="1" spans="1:8">
       <c r="A238" s="12" t="str">
-        <f>IF(G238&lt;&gt;"",UPPER(LEFT(G238,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G238,G238),"0000"),"")</f>
+        <f>IF(G238&lt;&gt;"",UPPER(LEFT(G238,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G238,G238),"0000"),"")</f>
         <v/>
       </c>
       <c r="B238" s="5"/>
@@ -4475,7 +4490,7 @@
     </row>
     <row r="239" customHeight="1" spans="1:8">
       <c r="A239" s="12" t="str">
-        <f>IF(G239&lt;&gt;"",UPPER(LEFT(G239,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G239,G239),"0000"),"")</f>
+        <f>IF(G239&lt;&gt;"",UPPER(LEFT(G239,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G239,G239),"0000"),"")</f>
         <v/>
       </c>
       <c r="B239" s="5"/>
@@ -4488,7 +4503,7 @@
     </row>
     <row r="240" customHeight="1" spans="1:8">
       <c r="A240" s="12" t="str">
-        <f>IF(G240&lt;&gt;"",UPPER(LEFT(G240,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G240,G240),"0000"),"")</f>
+        <f>IF(G240&lt;&gt;"",UPPER(LEFT(G240,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G240,G240),"0000"),"")</f>
         <v/>
       </c>
       <c r="B240" s="5"/>
@@ -4501,7 +4516,7 @@
     </row>
     <row r="241" customHeight="1" spans="1:8">
       <c r="A241" s="12" t="str">
-        <f>IF(G241&lt;&gt;"",UPPER(LEFT(G241,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G241,G241),"0000"),"")</f>
+        <f>IF(G241&lt;&gt;"",UPPER(LEFT(G241,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G241,G241),"0000"),"")</f>
         <v/>
       </c>
       <c r="B241" s="5"/>
@@ -4514,7 +4529,7 @@
     </row>
     <row r="242" customHeight="1" spans="1:8">
       <c r="A242" s="12" t="str">
-        <f>IF(G242&lt;&gt;"",UPPER(LEFT(G242,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G242,G242),"0000"),"")</f>
+        <f>IF(G242&lt;&gt;"",UPPER(LEFT(G242,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G242,G242),"0000"),"")</f>
         <v/>
       </c>
       <c r="B242" s="5"/>
@@ -4527,7 +4542,7 @@
     </row>
     <row r="243" customHeight="1" spans="1:8">
       <c r="A243" s="12" t="str">
-        <f>IF(G243&lt;&gt;"",UPPER(LEFT(G243,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G243,G243),"0000"),"")</f>
+        <f>IF(G243&lt;&gt;"",UPPER(LEFT(G243,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G243,G243),"0000"),"")</f>
         <v/>
       </c>
       <c r="B243" s="5"/>
@@ -4540,7 +4555,7 @@
     </row>
     <row r="244" customHeight="1" spans="1:8">
       <c r="A244" s="12" t="str">
-        <f>IF(G244&lt;&gt;"",UPPER(LEFT(G244,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G244,G244),"0000"),"")</f>
+        <f>IF(G244&lt;&gt;"",UPPER(LEFT(G244,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G244,G244),"0000"),"")</f>
         <v/>
       </c>
       <c r="B244" s="5"/>
@@ -4553,7 +4568,7 @@
     </row>
     <row r="245" customHeight="1" spans="1:8">
       <c r="A245" s="12" t="str">
-        <f>IF(G245&lt;&gt;"",UPPER(LEFT(G245,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G245,G245),"0000"),"")</f>
+        <f>IF(G245&lt;&gt;"",UPPER(LEFT(G245,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G245,G245),"0000"),"")</f>
         <v/>
       </c>
       <c r="B245" s="5"/>
@@ -4566,7 +4581,7 @@
     </row>
     <row r="246" customHeight="1" spans="1:8">
       <c r="A246" s="12" t="str">
-        <f>IF(G246&lt;&gt;"",UPPER(LEFT(G246,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G246,G246),"0000"),"")</f>
+        <f>IF(G246&lt;&gt;"",UPPER(LEFT(G246,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G246,G246),"0000"),"")</f>
         <v/>
       </c>
       <c r="B246" s="5"/>
@@ -4579,7 +4594,7 @@
     </row>
     <row r="247" customHeight="1" spans="1:8">
       <c r="A247" s="12" t="str">
-        <f>IF(G247&lt;&gt;"",UPPER(LEFT(G247,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G247,G247),"0000"),"")</f>
+        <f>IF(G247&lt;&gt;"",UPPER(LEFT(G247,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G247,G247),"0000"),"")</f>
         <v/>
       </c>
       <c r="B247" s="5"/>
@@ -4592,7 +4607,7 @@
     </row>
     <row r="248" customHeight="1" spans="1:8">
       <c r="A248" s="12" t="str">
-        <f>IF(G248&lt;&gt;"",UPPER(LEFT(G248,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G248,G248),"0000"),"")</f>
+        <f>IF(G248&lt;&gt;"",UPPER(LEFT(G248,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G248,G248),"0000"),"")</f>
         <v/>
       </c>
       <c r="B248" s="5"/>
@@ -4605,7 +4620,7 @@
     </row>
     <row r="249" customHeight="1" spans="1:8">
       <c r="A249" s="12" t="str">
-        <f>IF(G249&lt;&gt;"",UPPER(LEFT(G249,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G249,G249),"0000"),"")</f>
+        <f>IF(G249&lt;&gt;"",UPPER(LEFT(G249,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G249,G249),"0000"),"")</f>
         <v/>
       </c>
       <c r="B249" s="5"/>
@@ -4618,7 +4633,7 @@
     </row>
     <row r="250" customHeight="1" spans="1:8">
       <c r="A250" s="12" t="str">
-        <f>IF(G250&lt;&gt;"",UPPER(LEFT(G250,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G250,G250),"0000"),"")</f>
+        <f>IF(G250&lt;&gt;"",UPPER(LEFT(G250,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G250,G250),"0000"),"")</f>
         <v/>
       </c>
       <c r="B250" s="5"/>
@@ -4631,7 +4646,7 @@
     </row>
     <row r="251" customHeight="1" spans="1:8">
       <c r="A251" s="12" t="str">
-        <f>IF(G251&lt;&gt;"",UPPER(LEFT(G251,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G251,G251),"0000"),"")</f>
+        <f>IF(G251&lt;&gt;"",UPPER(LEFT(G251,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G251,G251),"0000"),"")</f>
         <v/>
       </c>
       <c r="B251" s="5"/>
@@ -4644,7 +4659,7 @@
     </row>
     <row r="252" customHeight="1" spans="1:8">
       <c r="A252" s="12" t="str">
-        <f>IF(G252&lt;&gt;"",UPPER(LEFT(G252,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G252,G252),"0000"),"")</f>
+        <f>IF(G252&lt;&gt;"",UPPER(LEFT(G252,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G252,G252),"0000"),"")</f>
         <v/>
       </c>
       <c r="B252" s="5"/>
@@ -4657,7 +4672,7 @@
     </row>
     <row r="253" customHeight="1" spans="1:8">
       <c r="A253" s="12" t="str">
-        <f>IF(G253&lt;&gt;"",UPPER(LEFT(G253,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G253,G253),"0000"),"")</f>
+        <f>IF(G253&lt;&gt;"",UPPER(LEFT(G253,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G253,G253),"0000"),"")</f>
         <v/>
       </c>
       <c r="B253" s="5"/>
@@ -4670,7 +4685,7 @@
     </row>
     <row r="254" customHeight="1" spans="1:8">
       <c r="A254" s="12" t="str">
-        <f>IF(G254&lt;&gt;"",UPPER(LEFT(G254,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G254,G254),"0000"),"")</f>
+        <f>IF(G254&lt;&gt;"",UPPER(LEFT(G254,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G254,G254),"0000"),"")</f>
         <v/>
       </c>
       <c r="B254" s="5"/>
@@ -4683,7 +4698,7 @@
     </row>
     <row r="255" customHeight="1" spans="1:8">
       <c r="A255" s="12" t="str">
-        <f>IF(G255&lt;&gt;"",UPPER(LEFT(G255,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G255,G255),"0000"),"")</f>
+        <f>IF(G255&lt;&gt;"",UPPER(LEFT(G255,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G255,G255),"0000"),"")</f>
         <v/>
       </c>
       <c r="B255" s="5"/>
@@ -4696,7 +4711,7 @@
     </row>
     <row r="256" customHeight="1" spans="1:8">
       <c r="A256" s="12" t="str">
-        <f>IF(G256&lt;&gt;"",UPPER(LEFT(G256,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G256,G256),"0000"),"")</f>
+        <f>IF(G256&lt;&gt;"",UPPER(LEFT(G256,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G256,G256),"0000"),"")</f>
         <v/>
       </c>
       <c r="B256" s="5"/>
@@ -4709,7 +4724,7 @@
     </row>
     <row r="257" customHeight="1" spans="1:8">
       <c r="A257" s="12" t="str">
-        <f>IF(G257&lt;&gt;"",UPPER(LEFT(G257,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G257,G257),"0000"),"")</f>
+        <f>IF(G257&lt;&gt;"",UPPER(LEFT(G257,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G257,G257),"0000"),"")</f>
         <v/>
       </c>
       <c r="B257" s="5"/>
@@ -4722,7 +4737,7 @@
     </row>
     <row r="258" customHeight="1" spans="1:8">
       <c r="A258" s="12" t="str">
-        <f>IF(G258&lt;&gt;"",UPPER(LEFT(G258,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G258,G258),"0000"),"")</f>
+        <f>IF(G258&lt;&gt;"",UPPER(LEFT(G258,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G258,G258),"0000"),"")</f>
         <v/>
       </c>
       <c r="B258" s="5"/>
@@ -4735,7 +4750,7 @@
     </row>
     <row r="259" customHeight="1" spans="1:8">
       <c r="A259" s="12" t="str">
-        <f>IF(G259&lt;&gt;"",UPPER(LEFT(G259,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G259,G259),"0000"),"")</f>
+        <f>IF(G259&lt;&gt;"",UPPER(LEFT(G259,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G259,G259),"0000"),"")</f>
         <v/>
       </c>
       <c r="B259" s="5"/>
@@ -4748,7 +4763,7 @@
     </row>
     <row r="260" customHeight="1" spans="1:8">
       <c r="A260" s="12" t="str">
-        <f>IF(G260&lt;&gt;"",UPPER(LEFT(G260,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G260,G260),"0000"),"")</f>
+        <f>IF(G260&lt;&gt;"",UPPER(LEFT(G260,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G260,G260),"0000"),"")</f>
         <v/>
       </c>
       <c r="B260" s="5"/>
@@ -4761,7 +4776,7 @@
     </row>
     <row r="261" customHeight="1" spans="1:8">
       <c r="A261" s="12" t="str">
-        <f>IF(G261&lt;&gt;"",UPPER(LEFT(G261,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G261,G261),"0000"),"")</f>
+        <f>IF(G261&lt;&gt;"",UPPER(LEFT(G261,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G261,G261),"0000"),"")</f>
         <v/>
       </c>
       <c r="B261" s="5"/>
@@ -4774,7 +4789,7 @@
     </row>
     <row r="262" customHeight="1" spans="1:8">
       <c r="A262" s="12" t="str">
-        <f>IF(G262&lt;&gt;"",UPPER(LEFT(G262,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G262,G262),"0000"),"")</f>
+        <f>IF(G262&lt;&gt;"",UPPER(LEFT(G262,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G262,G262),"0000"),"")</f>
         <v/>
       </c>
       <c r="B262" s="5"/>
@@ -4787,7 +4802,7 @@
     </row>
     <row r="263" customHeight="1" spans="1:8">
       <c r="A263" s="12" t="str">
-        <f>IF(G263&lt;&gt;"",UPPER(LEFT(G263,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G263,G263),"0000"),"")</f>
+        <f>IF(G263&lt;&gt;"",UPPER(LEFT(G263,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G263,G263),"0000"),"")</f>
         <v/>
       </c>
       <c r="B263" s="5"/>
@@ -4800,7 +4815,7 @@
     </row>
     <row r="264" customHeight="1" spans="1:8">
       <c r="A264" s="12" t="str">
-        <f>IF(G264&lt;&gt;"",UPPER(LEFT(G264,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G264,G264),"0000"),"")</f>
+        <f>IF(G264&lt;&gt;"",UPPER(LEFT(G264,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G264,G264),"0000"),"")</f>
         <v/>
       </c>
       <c r="B264" s="5"/>
@@ -4813,7 +4828,7 @@
     </row>
     <row r="265" customHeight="1" spans="1:8">
       <c r="A265" s="12" t="str">
-        <f>IF(G265&lt;&gt;"",UPPER(LEFT(G265,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G265,G265),"0000"),"")</f>
+        <f>IF(G265&lt;&gt;"",UPPER(LEFT(G265,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G265,G265),"0000"),"")</f>
         <v/>
       </c>
       <c r="B265" s="5"/>
@@ -4826,7 +4841,7 @@
     </row>
     <row r="266" customHeight="1" spans="1:8">
       <c r="A266" s="12" t="str">
-        <f>IF(G266&lt;&gt;"",UPPER(LEFT(G266,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G266,G266),"0000"),"")</f>
+        <f>IF(G266&lt;&gt;"",UPPER(LEFT(G266,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G266,G266),"0000"),"")</f>
         <v/>
       </c>
       <c r="B266" s="5"/>
@@ -4839,7 +4854,7 @@
     </row>
     <row r="267" customHeight="1" spans="1:8">
       <c r="A267" s="12" t="str">
-        <f>IF(G267&lt;&gt;"",UPPER(LEFT(G267,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G267,G267),"0000"),"")</f>
+        <f>IF(G267&lt;&gt;"",UPPER(LEFT(G267,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G267,G267),"0000"),"")</f>
         <v/>
       </c>
       <c r="B267" s="5"/>
@@ -4852,7 +4867,7 @@
     </row>
     <row r="268" customHeight="1" spans="1:8">
       <c r="A268" s="12" t="str">
-        <f>IF(G268&lt;&gt;"",UPPER(LEFT(G268,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G268,G268),"0000"),"")</f>
+        <f>IF(G268&lt;&gt;"",UPPER(LEFT(G268,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G268,G268),"0000"),"")</f>
         <v/>
       </c>
       <c r="B268" s="5"/>
@@ -4865,7 +4880,7 @@
     </row>
     <row r="269" customHeight="1" spans="1:8">
       <c r="A269" s="12" t="str">
-        <f>IF(G269&lt;&gt;"",UPPER(LEFT(G269,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G269,G269),"0000"),"")</f>
+        <f>IF(G269&lt;&gt;"",UPPER(LEFT(G269,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G269,G269),"0000"),"")</f>
         <v/>
       </c>
       <c r="B269" s="5"/>
@@ -4878,7 +4893,7 @@
     </row>
     <row r="270" customHeight="1" spans="1:8">
       <c r="A270" s="12" t="str">
-        <f>IF(G270&lt;&gt;"",UPPER(LEFT(G270,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G270,G270),"0000"),"")</f>
+        <f>IF(G270&lt;&gt;"",UPPER(LEFT(G270,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G270,G270),"0000"),"")</f>
         <v/>
       </c>
       <c r="B270" s="5"/>
@@ -4891,7 +4906,7 @@
     </row>
     <row r="271" customHeight="1" spans="1:8">
       <c r="A271" s="12" t="str">
-        <f>IF(G271&lt;&gt;"",UPPER(LEFT(G271,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G271,G271),"0000"),"")</f>
+        <f>IF(G271&lt;&gt;"",UPPER(LEFT(G271,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G271,G271),"0000"),"")</f>
         <v/>
       </c>
       <c r="B271" s="5"/>
@@ -4904,7 +4919,7 @@
     </row>
     <row r="272" customHeight="1" spans="1:8">
       <c r="A272" s="12" t="str">
-        <f>IF(G272&lt;&gt;"",UPPER(LEFT(G272,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G272,G272),"0000"),"")</f>
+        <f>IF(G272&lt;&gt;"",UPPER(LEFT(G272,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G272,G272),"0000"),"")</f>
         <v/>
       </c>
       <c r="B272" s="5"/>
@@ -4917,7 +4932,7 @@
     </row>
     <row r="273" customHeight="1" spans="1:8">
       <c r="A273" s="12" t="str">
-        <f>IF(G273&lt;&gt;"",UPPER(LEFT(G273,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G273,G273),"0000"),"")</f>
+        <f>IF(G273&lt;&gt;"",UPPER(LEFT(G273,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G273,G273),"0000"),"")</f>
         <v/>
       </c>
       <c r="B273" s="5"/>
@@ -4930,7 +4945,7 @@
     </row>
     <row r="274" customHeight="1" spans="1:8">
       <c r="A274" s="12" t="str">
-        <f>IF(G274&lt;&gt;"",UPPER(LEFT(G274,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G274,G274),"0000"),"")</f>
+        <f>IF(G274&lt;&gt;"",UPPER(LEFT(G274,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G274,G274),"0000"),"")</f>
         <v/>
       </c>
       <c r="B274" s="5"/>
@@ -4943,7 +4958,7 @@
     </row>
     <row r="275" customHeight="1" spans="1:8">
       <c r="A275" s="12" t="str">
-        <f>IF(G275&lt;&gt;"",UPPER(LEFT(G275,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G275,G275),"0000"),"")</f>
+        <f>IF(G275&lt;&gt;"",UPPER(LEFT(G275,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G275,G275),"0000"),"")</f>
         <v/>
       </c>
       <c r="B275" s="5"/>
@@ -4956,7 +4971,7 @@
     </row>
     <row r="276" customHeight="1" spans="1:8">
       <c r="A276" s="12" t="str">
-        <f>IF(G276&lt;&gt;"",UPPER(LEFT(G276,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G276,G276),"0000"),"")</f>
+        <f>IF(G276&lt;&gt;"",UPPER(LEFT(G276,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G276,G276),"0000"),"")</f>
         <v/>
       </c>
       <c r="B276" s="5"/>
@@ -4969,7 +4984,7 @@
     </row>
     <row r="277" customHeight="1" spans="1:8">
       <c r="A277" s="12" t="str">
-        <f>IF(G277&lt;&gt;"",UPPER(LEFT(G277,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G277,G277),"0000"),"")</f>
+        <f>IF(G277&lt;&gt;"",UPPER(LEFT(G277,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G277,G277),"0000"),"")</f>
         <v/>
       </c>
       <c r="B277" s="5"/>
@@ -4982,7 +4997,7 @@
     </row>
     <row r="278" customHeight="1" spans="1:8">
       <c r="A278" s="12" t="str">
-        <f>IF(G278&lt;&gt;"",UPPER(LEFT(G278,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G278,G278),"0000"),"")</f>
+        <f>IF(G278&lt;&gt;"",UPPER(LEFT(G278,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G278,G278),"0000"),"")</f>
         <v/>
       </c>
       <c r="B278" s="5"/>
@@ -4995,7 +5010,7 @@
     </row>
     <row r="279" customHeight="1" spans="1:8">
       <c r="A279" s="12" t="str">
-        <f>IF(G279&lt;&gt;"",UPPER(LEFT(G279,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G279,G279),"0000"),"")</f>
+        <f>IF(G279&lt;&gt;"",UPPER(LEFT(G279,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G279,G279),"0000"),"")</f>
         <v/>
       </c>
       <c r="B279" s="5"/>
@@ -5008,7 +5023,7 @@
     </row>
     <row r="280" customHeight="1" spans="1:8">
       <c r="A280" s="12" t="str">
-        <f>IF(G280&lt;&gt;"",UPPER(LEFT(G280,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G280,G280),"0000"),"")</f>
+        <f>IF(G280&lt;&gt;"",UPPER(LEFT(G280,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G280,G280),"0000"),"")</f>
         <v/>
       </c>
       <c r="B280" s="5"/>
@@ -5021,7 +5036,7 @@
     </row>
     <row r="281" customHeight="1" spans="1:8">
       <c r="A281" s="12" t="str">
-        <f>IF(G281&lt;&gt;"",UPPER(LEFT(G281,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G281,G281),"0000"),"")</f>
+        <f>IF(G281&lt;&gt;"",UPPER(LEFT(G281,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G281,G281),"0000"),"")</f>
         <v/>
       </c>
       <c r="B281" s="5"/>
@@ -5034,7 +5049,7 @@
     </row>
     <row r="282" customHeight="1" spans="1:8">
       <c r="A282" s="12" t="str">
-        <f>IF(G282&lt;&gt;"",UPPER(LEFT(G282,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G282,G282),"0000"),"")</f>
+        <f>IF(G282&lt;&gt;"",UPPER(LEFT(G282,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G282,G282),"0000"),"")</f>
         <v/>
       </c>
       <c r="B282" s="5"/>
@@ -5047,7 +5062,7 @@
     </row>
     <row r="283" customHeight="1" spans="1:8">
       <c r="A283" s="12" t="str">
-        <f>IF(G283&lt;&gt;"",UPPER(LEFT(G283,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G283,G283),"0000"),"")</f>
+        <f>IF(G283&lt;&gt;"",UPPER(LEFT(G283,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G283,G283),"0000"),"")</f>
         <v/>
       </c>
       <c r="B283" s="5"/>
@@ -5060,7 +5075,7 @@
     </row>
     <row r="284" customHeight="1" spans="1:8">
       <c r="A284" s="12" t="str">
-        <f>IF(G284&lt;&gt;"",UPPER(LEFT(G284,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G284,G284),"0000"),"")</f>
+        <f>IF(G284&lt;&gt;"",UPPER(LEFT(G284,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G284,G284),"0000"),"")</f>
         <v/>
       </c>
       <c r="B284" s="5"/>
@@ -5073,7 +5088,7 @@
     </row>
     <row r="285" customHeight="1" spans="1:8">
       <c r="A285" s="12" t="str">
-        <f>IF(G285&lt;&gt;"",UPPER(LEFT(G285,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G285,G285),"0000"),"")</f>
+        <f>IF(G285&lt;&gt;"",UPPER(LEFT(G285,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G285,G285),"0000"),"")</f>
         <v/>
       </c>
       <c r="B285" s="5"/>
@@ -5086,7 +5101,7 @@
     </row>
     <row r="286" customHeight="1" spans="1:8">
       <c r="A286" s="12" t="str">
-        <f>IF(G286&lt;&gt;"",UPPER(LEFT(G286,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G286,G286),"0000"),"")</f>
+        <f>IF(G286&lt;&gt;"",UPPER(LEFT(G286,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G286,G286),"0000"),"")</f>
         <v/>
       </c>
       <c r="B286" s="5"/>
@@ -5099,7 +5114,7 @@
     </row>
     <row r="287" customHeight="1" spans="1:8">
       <c r="A287" s="12" t="str">
-        <f>IF(G287&lt;&gt;"",UPPER(LEFT(G287,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G287,G287),"0000"),"")</f>
+        <f>IF(G287&lt;&gt;"",UPPER(LEFT(G287,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G287,G287),"0000"),"")</f>
         <v/>
       </c>
       <c r="B287" s="5"/>
@@ -5112,7 +5127,7 @@
     </row>
     <row r="288" customHeight="1" spans="1:8">
       <c r="A288" s="12" t="str">
-        <f>IF(G288&lt;&gt;"",UPPER(LEFT(G288,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G288,G288),"0000"),"")</f>
+        <f>IF(G288&lt;&gt;"",UPPER(LEFT(G288,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G288,G288),"0000"),"")</f>
         <v/>
       </c>
       <c r="B288" s="5"/>
@@ -5125,7 +5140,7 @@
     </row>
     <row r="289" customHeight="1" spans="1:8">
       <c r="A289" s="12" t="str">
-        <f>IF(G289&lt;&gt;"",UPPER(LEFT(G289,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G289,G289),"0000"),"")</f>
+        <f>IF(G289&lt;&gt;"",UPPER(LEFT(G289,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G289,G289),"0000"),"")</f>
         <v/>
       </c>
       <c r="B289" s="5"/>
@@ -5138,7 +5153,7 @@
     </row>
     <row r="290" customHeight="1" spans="1:8">
       <c r="A290" s="12" t="str">
-        <f>IF(G290&lt;&gt;"",UPPER(LEFT(G290,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G290,G290),"0000"),"")</f>
+        <f>IF(G290&lt;&gt;"",UPPER(LEFT(G290,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G290,G290),"0000"),"")</f>
         <v/>
       </c>
       <c r="B290" s="5"/>
@@ -5151,7 +5166,7 @@
     </row>
     <row r="291" customHeight="1" spans="1:8">
       <c r="A291" s="12" t="str">
-        <f>IF(G291&lt;&gt;"",UPPER(LEFT(G291,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G291,G291),"0000"),"")</f>
+        <f>IF(G291&lt;&gt;"",UPPER(LEFT(G291,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G291,G291),"0000"),"")</f>
         <v/>
       </c>
       <c r="B291" s="5"/>
@@ -5164,7 +5179,7 @@
     </row>
     <row r="292" customHeight="1" spans="1:8">
       <c r="A292" s="12" t="str">
-        <f>IF(G292&lt;&gt;"",UPPER(LEFT(G292,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G292,G292),"0000"),"")</f>
+        <f>IF(G292&lt;&gt;"",UPPER(LEFT(G292,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G292,G292),"0000"),"")</f>
         <v/>
       </c>
       <c r="B292" s="5"/>
@@ -5177,7 +5192,7 @@
     </row>
     <row r="293" customHeight="1" spans="1:8">
       <c r="A293" s="12" t="str">
-        <f>IF(G293&lt;&gt;"",UPPER(LEFT(G293,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G293,G293),"0000"),"")</f>
+        <f>IF(G293&lt;&gt;"",UPPER(LEFT(G293,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G293,G293),"0000"),"")</f>
         <v/>
       </c>
       <c r="B293" s="5"/>
@@ -5190,7 +5205,7 @@
     </row>
     <row r="294" customHeight="1" spans="1:8">
       <c r="A294" s="12" t="str">
-        <f>IF(G294&lt;&gt;"",UPPER(LEFT(G294,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G294,G294),"0000"),"")</f>
+        <f>IF(G294&lt;&gt;"",UPPER(LEFT(G294,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G294,G294),"0000"),"")</f>
         <v/>
       </c>
       <c r="B294" s="5"/>
@@ -5203,7 +5218,7 @@
     </row>
     <row r="295" customHeight="1" spans="1:8">
       <c r="A295" s="12" t="str">
-        <f>IF(G295&lt;&gt;"",UPPER(LEFT(G295,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G295,G295),"0000"),"")</f>
+        <f>IF(G295&lt;&gt;"",UPPER(LEFT(G295,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G295,G295),"0000"),"")</f>
         <v/>
       </c>
       <c r="B295" s="5"/>
@@ -5216,7 +5231,7 @@
     </row>
     <row r="296" customHeight="1" spans="1:8">
       <c r="A296" s="12" t="str">
-        <f>IF(G296&lt;&gt;"",UPPER(LEFT(G296,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G296,G296),"0000"),"")</f>
+        <f>IF(G296&lt;&gt;"",UPPER(LEFT(G296,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G296,G296),"0000"),"")</f>
         <v/>
       </c>
       <c r="B296" s="5"/>
@@ -5229,7 +5244,7 @@
     </row>
     <row r="297" customHeight="1" spans="1:8">
       <c r="A297" s="12" t="str">
-        <f>IF(G297&lt;&gt;"",UPPER(LEFT(G297,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G297,G297),"0000"),"")</f>
+        <f>IF(G297&lt;&gt;"",UPPER(LEFT(G297,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G297,G297),"0000"),"")</f>
         <v/>
       </c>
       <c r="B297" s="5"/>
@@ -5242,7 +5257,7 @@
     </row>
     <row r="298" customHeight="1" spans="1:8">
       <c r="A298" s="12" t="str">
-        <f>IF(G298&lt;&gt;"",UPPER(LEFT(G298,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G298,G298),"0000"),"")</f>
+        <f>IF(G298&lt;&gt;"",UPPER(LEFT(G298,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G298,G298),"0000"),"")</f>
         <v/>
       </c>
       <c r="B298" s="5"/>
@@ -5255,7 +5270,7 @@
     </row>
     <row r="299" customHeight="1" spans="1:8">
       <c r="A299" s="12" t="str">
-        <f>IF(G299&lt;&gt;"",UPPER(LEFT(G299,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G299,G299),"0000"),"")</f>
+        <f>IF(G299&lt;&gt;"",UPPER(LEFT(G299,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G299,G299),"0000"),"")</f>
         <v/>
       </c>
       <c r="B299" s="5"/>
@@ -5268,7 +5283,7 @@
     </row>
     <row r="300" customHeight="1" spans="1:8">
       <c r="A300" s="12" t="str">
-        <f>IF(G300&lt;&gt;"",UPPER(LEFT(G300,1))&amp;"-"&amp;TEXT('Import time'!$B$1,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G300,G300),"0000"),"")</f>
+        <f>IF(G300&lt;&gt;"",UPPER(LEFT(G300,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G300,G300),"0000"),"")</f>
         <v/>
       </c>
       <c r="B300" s="5"/>
@@ -5309,8 +5324,8 @@
   </sheetPr>
   <dimension ref="A1:K1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6296296296296" defaultRowHeight="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
[0406] Fix Template Cow Import.xlsx
</commit_message>
<xml_diff>
--- a/src/main/resources/static/document/Template Cow Import.xlsx
+++ b/src/main/resources/static/document/Template Cow Import.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9000"/>
+    <workbookView windowWidth="23040" windowHeight="9000" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Import time" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="45">
   <si>
     <t>Import time(s)</t>
   </si>
@@ -62,6 +62,18 @@
   </si>
   <si>
     <t>Description</t>
+  </si>
+  <si>
+    <t>youngCow</t>
+  </si>
+  <si>
+    <t>european</t>
+  </si>
+  <si>
+    <t>female</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Holstein Friesian </t>
   </si>
   <si>
     <t>Cow Name</t>
@@ -121,13 +133,7 @@
     <t>seriousSickcow</t>
   </si>
   <si>
-    <t>youngCow</t>
-  </si>
-  <si>
     <t>culling</t>
-  </si>
-  <si>
-    <t>european</t>
   </si>
   <si>
     <t>indian</t>
@@ -151,13 +157,7 @@
     <t>crossbreed</t>
   </si>
   <si>
-    <t>female</t>
-  </si>
-  <si>
     <t>male</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Holstein Friesian </t>
   </si>
   <si>
     <t>Ayrshire</t>
@@ -1342,8 +1342,8 @@
   </sheetPr>
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6296296296296" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1"/>
@@ -1354,7 +1354,9 @@
       </c>
     </row>
     <row r="2" customHeight="1" spans="1:1">
-      <c r="A2" s="15"/>
+      <c r="A2" s="15">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1370,7 +1372,7 @@
   <dimension ref="A1:K300"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6296296296296" defaultRowHeight="15.75" customHeight="1"/>
@@ -1407,14 +1409,26 @@
     <row r="2" customHeight="1" spans="1:8">
       <c r="A2" s="12" t="str">
         <f>IF(G2&lt;&gt;"",UPPER(LEFT(G2,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G2,G2),"0000"),"")</f>
-        <v/>
-      </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
+        <v>H-0001-0001</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="13">
+        <v>45755</v>
+      </c>
+      <c r="D2" s="13">
+        <v>45755</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="H2" s="5"/>
     </row>
     <row r="3" customHeight="1" spans="1:8">
@@ -5324,8 +5338,8 @@
   </sheetPr>
   <dimension ref="A1:K1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6296296296296" defaultRowHeight="15.75" customHeight="1"/>
@@ -5338,34 +5352,34 @@
   <sheetData>
     <row r="1" customHeight="1" spans="1:11">
       <c r="A1" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="J1" s="9" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>8</v>
@@ -5374,17 +5388,35 @@
     <row r="2" customHeight="1" spans="1:11">
       <c r="A2" s="5" t="str">
         <f>Cow!A2</f>
-        <v/>
-      </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
+        <v>H-0001-0001</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="6">
+        <v>38</v>
+      </c>
+      <c r="F2" s="6">
+        <v>65</v>
+      </c>
+      <c r="G2" s="6">
+        <v>30</v>
+      </c>
+      <c r="H2" s="6">
+        <v>60</v>
+      </c>
+      <c r="I2" s="7">
+        <v>1.85</v>
+      </c>
+      <c r="J2" s="7">
+        <v>1.9</v>
+      </c>
       <c r="K2" s="5"/>
     </row>
     <row r="3" customHeight="1" spans="1:11">
@@ -16487,27 +16519,27 @@
   <sheetData>
     <row r="1" customHeight="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" customHeight="1" spans="1:1">
       <c r="A2" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:1">
       <c r="A3" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" customHeight="1" spans="1:1">
       <c r="A4" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" customHeight="1" spans="1:1">
       <c r="A5" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -16531,32 +16563,32 @@
   <sheetData>
     <row r="1" customHeight="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" customHeight="1" spans="1:1">
       <c r="A2" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:1">
       <c r="A3" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" customHeight="1" spans="1:1">
       <c r="A4" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" customHeight="1" spans="1:1">
       <c r="A5" s="1" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" customHeight="1" spans="1:1">
       <c r="A6" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -16580,32 +16612,32 @@
   <sheetData>
     <row r="2" customHeight="1" spans="1:1">
       <c r="A2" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:1">
       <c r="A3" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" customHeight="1" spans="1:1">
       <c r="A4" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" customHeight="1" spans="1:1">
       <c r="A5" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" customHeight="1" spans="1:1">
       <c r="A6" s="1" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" customHeight="1" spans="1:1">
       <c r="A7" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -16629,42 +16661,42 @@
   <sheetData>
     <row r="1" customHeight="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" customHeight="1" spans="1:1">
       <c r="A2" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:1">
       <c r="A3" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" customHeight="1" spans="1:1">
       <c r="A4" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" customHeight="1" spans="1:1">
       <c r="A5" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" customHeight="1" spans="1:1">
       <c r="A6" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" customHeight="1" spans="1:1">
       <c r="A7" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" customHeight="1" spans="1:1">
       <c r="A8" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -16688,12 +16720,12 @@
   <sheetData>
     <row r="1" customHeight="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" customHeight="1" spans="1:1">
       <c r="A2" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -16717,7 +16749,7 @@
   <sheetData>
     <row r="1" customHeight="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" customHeight="1" spans="1:1">

</xml_diff>

<commit_message>
[0412] Fix Template Cow Import
</commit_message>
<xml_diff>
--- a/src/main/resources/static/document/Template Cow Import.xlsx
+++ b/src/main/resources/static/document/Template Cow Import.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9000" activeTab="2"/>
+    <workbookView windowWidth="23040" windowHeight="9000" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Import time" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="45">
   <si>
     <t>Import time(s)</t>
   </si>
@@ -74,6 +74,9 @@
   </si>
   <si>
     <t xml:space="preserve">Holstein Friesian </t>
+  </si>
+  <si>
+    <t>Ayrshire</t>
   </si>
   <si>
     <t>Cow Name</t>
@@ -158,9 +161,6 @@
   </si>
   <si>
     <t>male</t>
-  </si>
-  <si>
-    <t>Ayrshire</t>
   </si>
   <si>
     <t>Guernsey</t>
@@ -1371,8 +1371,8 @@
   </sheetPr>
   <dimension ref="A1:K300"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6296296296296" defaultRowHeight="15.75" customHeight="1"/>
@@ -1434,14 +1434,16 @@
     <row r="3" customHeight="1" spans="1:8">
       <c r="A3" s="12" t="str">
         <f>IF(G3&lt;&gt;"",UPPER(LEFT(G3,1))&amp;"-"&amp;TEXT('Import time'!$A$2,"0000")&amp;"-"&amp;TEXT(COUNTIF($G$2:G3,G3),"0000"),"")</f>
-        <v/>
+        <v>A-0001-0001</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="13"/>
       <c r="D3" s="13"/>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
+      <c r="G3" s="6" t="s">
+        <v>13</v>
+      </c>
       <c r="H3" s="5"/>
     </row>
     <row r="4" customHeight="1" spans="1:8">
@@ -5338,7 +5340,7 @@
   </sheetPr>
   <dimension ref="A1:K1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
@@ -5352,34 +5354,34 @@
   <sheetData>
     <row r="1" customHeight="1" spans="1:11">
       <c r="A1" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J1" s="9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>8</v>
@@ -5391,7 +5393,7 @@
         <v>H-0001-0001</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C2" s="7">
         <v>1.5</v>
@@ -5422,7 +5424,7 @@
     <row r="3" customHeight="1" spans="1:11">
       <c r="A3" s="5" t="str">
         <f>Cow!A3</f>
-        <v/>
+        <v>A-0001-0001</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="7"/>
@@ -16519,27 +16521,27 @@
   <sheetData>
     <row r="1" customHeight="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" customHeight="1" spans="1:1">
       <c r="A2" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:1">
       <c r="A3" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" customHeight="1" spans="1:1">
       <c r="A4" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" customHeight="1" spans="1:1">
       <c r="A5" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -16563,22 +16565,22 @@
   <sheetData>
     <row r="1" customHeight="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" customHeight="1" spans="1:1">
       <c r="A2" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:1">
       <c r="A3" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" customHeight="1" spans="1:1">
       <c r="A4" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" customHeight="1" spans="1:1">
@@ -16588,7 +16590,7 @@
     </row>
     <row r="6" customHeight="1" spans="1:1">
       <c r="A6" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -16612,22 +16614,22 @@
   <sheetData>
     <row r="2" customHeight="1" spans="1:1">
       <c r="A2" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:1">
       <c r="A3" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" customHeight="1" spans="1:1">
       <c r="A4" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" customHeight="1" spans="1:1">
       <c r="A5" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" customHeight="1" spans="1:1">
@@ -16637,7 +16639,7 @@
     </row>
     <row r="7" customHeight="1" spans="1:1">
       <c r="A7" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -16666,37 +16668,37 @@
     </row>
     <row r="2" customHeight="1" spans="1:1">
       <c r="A2" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:1">
       <c r="A3" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" customHeight="1" spans="1:1">
       <c r="A4" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" customHeight="1" spans="1:1">
       <c r="A5" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" customHeight="1" spans="1:1">
       <c r="A6" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" customHeight="1" spans="1:1">
       <c r="A7" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" customHeight="1" spans="1:1">
       <c r="A8" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -16725,7 +16727,7 @@
     </row>
     <row r="2" customHeight="1" spans="1:1">
       <c r="A2" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -16754,7 +16756,7 @@
     </row>
     <row r="2" customHeight="1" spans="1:1">
       <c r="A2" s="1" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:1">

</xml_diff>